<commit_message>
added ts function, fixed bugs
</commit_message>
<xml_diff>
--- a/example/kerber_landnetz_fl2/topology.xlsx
+++ b/example/kerber_landnetz_fl2/topology.xlsx
@@ -8,9 +8,9 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Users/chujiahe/Desktop/propens-pandapower/example/kerber_landnetz_fl2/"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{25C78155-3D0D-1946-A942-762057512A9F}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{07910476-1E04-6B4F-A79E-9D4E7F4DBD8C}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="0" yWindow="640" windowWidth="30240" windowHeight="17600" activeTab="8" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="3200" yWindow="1240" windowWidth="30240" windowHeight="17600" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="parameters" sheetId="1" r:id="rId1"/>
@@ -723,6 +723,55 @@
     </ext>
   </extLst>
 </styleSheet>
+</file>
+
+<file path=xl/drawings/drawing1.xml><?xml version="1.0" encoding="utf-8"?>
+<xdr:wsDr xmlns:xdr="http://schemas.openxmlformats.org/drawingml/2006/spreadsheetDrawing" xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main">
+  <xdr:twoCellAnchor editAs="oneCell">
+    <xdr:from>
+      <xdr:col>8</xdr:col>
+      <xdr:colOff>508000</xdr:colOff>
+      <xdr:row>4</xdr:row>
+      <xdr:rowOff>0</xdr:rowOff>
+    </xdr:from>
+    <xdr:to>
+      <xdr:col>17</xdr:col>
+      <xdr:colOff>88900</xdr:colOff>
+      <xdr:row>37</xdr:row>
+      <xdr:rowOff>12700</xdr:rowOff>
+    </xdr:to>
+    <xdr:pic>
+      <xdr:nvPicPr>
+        <xdr:cNvPr id="2" name="Picture 1">
+          <a:extLst>
+            <a:ext uri="{FF2B5EF4-FFF2-40B4-BE49-F238E27FC236}">
+              <a16:creationId xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" id="{F7E5573B-D761-A932-A6E8-1E508F8F9D9A}"/>
+            </a:ext>
+          </a:extLst>
+        </xdr:cNvPr>
+        <xdr:cNvPicPr>
+          <a:picLocks noChangeAspect="1"/>
+        </xdr:cNvPicPr>
+      </xdr:nvPicPr>
+      <xdr:blipFill>
+        <a:blip xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" r:embed="rId1"/>
+        <a:stretch>
+          <a:fillRect/>
+        </a:stretch>
+      </xdr:blipFill>
+      <xdr:spPr>
+        <a:xfrm>
+          <a:off x="5892800" y="762000"/>
+          <a:ext cx="5638800" cy="6299200"/>
+        </a:xfrm>
+        <a:prstGeom prst="rect">
+          <a:avLst/>
+        </a:prstGeom>
+      </xdr:spPr>
+    </xdr:pic>
+    <xdr:clientData/>
+  </xdr:twoCellAnchor>
+</xdr:wsDr>
 </file>
 
 <file path=xl/theme/theme1.xml><?xml version="1.0" encoding="utf-8"?>
@@ -1048,8 +1097,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
   <dimension ref="A1:H2"/>
   <sheetViews>
-    <sheetView workbookViewId="0">
-      <selection activeCell="N16" sqref="N16"/>
+    <sheetView tabSelected="1" workbookViewId="0">
+      <selection activeCell="U16" sqref="U16"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultColWidth="8.83203125" defaultRowHeight="15" x14ac:dyDescent="0.2"/>
@@ -1099,6 +1148,7 @@
     </row>
   </sheetData>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
+  <drawing r:id="rId1"/>
 </worksheet>
 </file>
 
@@ -3596,7 +3646,7 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0B00-000000000000}">
   <dimension ref="A1:D156"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="A117" workbookViewId="0">
+    <sheetView topLeftCell="A117" workbookViewId="0">
       <selection activeCell="G26" sqref="G26"/>
     </sheetView>
   </sheetViews>

</xml_diff>

<commit_message>
testing and plotting done, kerber netz with geodata
</commit_message>
<xml_diff>
--- a/example/kerber_landnetz_fl2/topology.xlsx
+++ b/example/kerber_landnetz_fl2/topology.xlsx
@@ -1,16 +1,16 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="4" rupBuild="11211"/>
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="4" rupBuild="26026"/>
   <workbookPr defaultThemeVersion="124226"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Users/chujiahe/Desktop/propens-pandapower/example/kerber_landnetz_fl2/"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\marti\OneDrive - TUM\projects\propens-pandapower\example\kerber_landnetz_fl2\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{A26B2D76-04CB-4048-9C11-FB1EE9093B0A}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{92D3299F-56BC-49B1-9767-E79B1C4B9502}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="0" yWindow="640" windowWidth="30240" windowHeight="17600" activeTab="9" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="-108" yWindow="-108" windowWidth="23256" windowHeight="12456" activeTab="7" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="parameters" sheetId="1" r:id="rId1"/>
@@ -864,7 +864,7 @@
 </file>
 
 <file path=xl/theme/theme1.xml><?xml version="1.0" encoding="utf-8"?>
-<a:theme xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main" name="Office Theme 2013 - 2022">
+<a:theme xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main" name="Office Theme">
   <a:themeElements>
     <a:clrScheme name="Office">
       <a:dk1>
@@ -1190,9 +1190,9 @@
       <selection activeCell="S30" sqref="S30"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr baseColWidth="10" defaultColWidth="8.83203125" defaultRowHeight="15" x14ac:dyDescent="0.2"/>
+  <sheetFormatPr defaultColWidth="8.77734375" defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
   <sheetData>
-    <row r="1" spans="1:7" x14ac:dyDescent="0.2">
+    <row r="1" spans="1:7" x14ac:dyDescent="0.3">
       <c r="B1" s="1" t="s">
         <v>0</v>
       </c>
@@ -1212,7 +1212,7 @@
         <v>5</v>
       </c>
     </row>
-    <row r="2" spans="1:7" x14ac:dyDescent="0.2">
+    <row r="2" spans="1:7" x14ac:dyDescent="0.3">
       <c r="A2" s="1">
         <v>0</v>
       </c>
@@ -1242,13 +1242,13 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{39D2056C-370F-E94D-8820-25D0D7A823B9}">
   <dimension ref="A1:D232"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="A203" workbookViewId="0">
-      <selection activeCell="R236" sqref="R236"/>
+    <sheetView topLeftCell="A203" workbookViewId="0">
+      <selection activeCell="I221" sqref="I221"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr baseColWidth="10" defaultColWidth="8.83203125" defaultRowHeight="15" x14ac:dyDescent="0.2"/>
+  <sheetFormatPr defaultColWidth="8.77734375" defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
   <sheetData>
-    <row r="1" spans="1:4" x14ac:dyDescent="0.2">
+    <row r="1" spans="1:4" x14ac:dyDescent="0.3">
       <c r="B1" s="1" t="s">
         <v>52</v>
       </c>
@@ -1259,7 +1259,7 @@
         <v>201</v>
       </c>
     </row>
-    <row r="2" spans="1:4" x14ac:dyDescent="0.2">
+    <row r="2" spans="1:4" x14ac:dyDescent="0.3">
       <c r="A2" s="1">
         <v>0</v>
       </c>
@@ -1273,7 +1273,7 @@
         <v>220</v>
       </c>
     </row>
-    <row r="3" spans="1:4" x14ac:dyDescent="0.2">
+    <row r="3" spans="1:4" x14ac:dyDescent="0.3">
       <c r="A3" s="1">
         <v>1</v>
       </c>
@@ -1287,7 +1287,7 @@
         <v>221</v>
       </c>
     </row>
-    <row r="4" spans="1:4" x14ac:dyDescent="0.2">
+    <row r="4" spans="1:4" x14ac:dyDescent="0.3">
       <c r="A4" s="1">
         <v>2</v>
       </c>
@@ -1301,7 +1301,7 @@
         <v>220</v>
       </c>
     </row>
-    <row r="5" spans="1:4" x14ac:dyDescent="0.2">
+    <row r="5" spans="1:4" x14ac:dyDescent="0.3">
       <c r="A5" s="1">
         <v>3</v>
       </c>
@@ -1315,7 +1315,7 @@
         <v>220</v>
       </c>
     </row>
-    <row r="6" spans="1:4" x14ac:dyDescent="0.2">
+    <row r="6" spans="1:4" x14ac:dyDescent="0.3">
       <c r="A6" s="1">
         <v>4</v>
       </c>
@@ -1329,7 +1329,7 @@
         <v>222</v>
       </c>
     </row>
-    <row r="7" spans="1:4" x14ac:dyDescent="0.2">
+    <row r="7" spans="1:4" x14ac:dyDescent="0.3">
       <c r="A7" s="1">
         <v>5</v>
       </c>
@@ -1343,7 +1343,7 @@
         <v>220</v>
       </c>
     </row>
-    <row r="8" spans="1:4" x14ac:dyDescent="0.2">
+    <row r="8" spans="1:4" x14ac:dyDescent="0.3">
       <c r="A8" s="1">
         <v>6</v>
       </c>
@@ -1357,7 +1357,7 @@
         <v>223</v>
       </c>
     </row>
-    <row r="9" spans="1:4" x14ac:dyDescent="0.2">
+    <row r="9" spans="1:4" x14ac:dyDescent="0.3">
       <c r="A9" s="1">
         <v>7</v>
       </c>
@@ -1371,7 +1371,7 @@
         <v>221</v>
       </c>
     </row>
-    <row r="10" spans="1:4" x14ac:dyDescent="0.2">
+    <row r="10" spans="1:4" x14ac:dyDescent="0.3">
       <c r="A10" s="1">
         <v>8</v>
       </c>
@@ -1385,7 +1385,7 @@
         <v>221</v>
       </c>
     </row>
-    <row r="11" spans="1:4" x14ac:dyDescent="0.2">
+    <row r="11" spans="1:4" x14ac:dyDescent="0.3">
       <c r="A11" s="1">
         <v>9</v>
       </c>
@@ -1399,7 +1399,7 @@
         <v>221</v>
       </c>
     </row>
-    <row r="12" spans="1:4" x14ac:dyDescent="0.2">
+    <row r="12" spans="1:4" x14ac:dyDescent="0.3">
       <c r="A12" s="1">
         <v>10</v>
       </c>
@@ -1413,7 +1413,7 @@
         <v>221</v>
       </c>
     </row>
-    <row r="13" spans="1:4" x14ac:dyDescent="0.2">
+    <row r="13" spans="1:4" x14ac:dyDescent="0.3">
       <c r="A13" s="1">
         <v>11</v>
       </c>
@@ -1427,7 +1427,7 @@
         <v>221</v>
       </c>
     </row>
-    <row r="14" spans="1:4" x14ac:dyDescent="0.2">
+    <row r="14" spans="1:4" x14ac:dyDescent="0.3">
       <c r="A14" s="1">
         <v>12</v>
       </c>
@@ -1441,7 +1441,7 @@
         <v>221</v>
       </c>
     </row>
-    <row r="15" spans="1:4" x14ac:dyDescent="0.2">
+    <row r="15" spans="1:4" x14ac:dyDescent="0.3">
       <c r="A15" s="1">
         <v>13</v>
       </c>
@@ -1455,7 +1455,7 @@
         <v>222</v>
       </c>
     </row>
-    <row r="16" spans="1:4" x14ac:dyDescent="0.2">
+    <row r="16" spans="1:4" x14ac:dyDescent="0.3">
       <c r="A16" s="1">
         <v>14</v>
       </c>
@@ -1469,7 +1469,7 @@
         <v>220</v>
       </c>
     </row>
-    <row r="17" spans="1:4" x14ac:dyDescent="0.2">
+    <row r="17" spans="1:4" x14ac:dyDescent="0.3">
       <c r="A17" s="1">
         <v>15</v>
       </c>
@@ -1483,7 +1483,7 @@
         <v>220</v>
       </c>
     </row>
-    <row r="18" spans="1:4" x14ac:dyDescent="0.2">
+    <row r="18" spans="1:4" x14ac:dyDescent="0.3">
       <c r="A18" s="1">
         <v>16</v>
       </c>
@@ -1497,7 +1497,7 @@
         <v>224</v>
       </c>
     </row>
-    <row r="19" spans="1:4" x14ac:dyDescent="0.2">
+    <row r="19" spans="1:4" x14ac:dyDescent="0.3">
       <c r="A19" s="1">
         <v>17</v>
       </c>
@@ -1511,7 +1511,7 @@
         <v>221</v>
       </c>
     </row>
-    <row r="20" spans="1:4" x14ac:dyDescent="0.2">
+    <row r="20" spans="1:4" x14ac:dyDescent="0.3">
       <c r="A20" s="1">
         <v>18</v>
       </c>
@@ -1525,7 +1525,7 @@
         <v>221</v>
       </c>
     </row>
-    <row r="21" spans="1:4" x14ac:dyDescent="0.2">
+    <row r="21" spans="1:4" x14ac:dyDescent="0.3">
       <c r="A21" s="1">
         <v>19</v>
       </c>
@@ -1539,7 +1539,7 @@
         <v>221</v>
       </c>
     </row>
-    <row r="22" spans="1:4" x14ac:dyDescent="0.2">
+    <row r="22" spans="1:4" x14ac:dyDescent="0.3">
       <c r="A22" s="1">
         <v>20</v>
       </c>
@@ -1553,7 +1553,7 @@
         <v>221</v>
       </c>
     </row>
-    <row r="23" spans="1:4" x14ac:dyDescent="0.2">
+    <row r="23" spans="1:4" x14ac:dyDescent="0.3">
       <c r="A23" s="1">
         <v>21</v>
       </c>
@@ -1567,7 +1567,7 @@
         <v>222</v>
       </c>
     </row>
-    <row r="24" spans="1:4" x14ac:dyDescent="0.2">
+    <row r="24" spans="1:4" x14ac:dyDescent="0.3">
       <c r="A24" s="1">
         <v>22</v>
       </c>
@@ -1581,7 +1581,7 @@
         <v>220</v>
       </c>
     </row>
-    <row r="25" spans="1:4" x14ac:dyDescent="0.2">
+    <row r="25" spans="1:4" x14ac:dyDescent="0.3">
       <c r="A25" s="1">
         <v>23</v>
       </c>
@@ -1595,7 +1595,7 @@
         <v>222</v>
       </c>
     </row>
-    <row r="26" spans="1:4" x14ac:dyDescent="0.2">
+    <row r="26" spans="1:4" x14ac:dyDescent="0.3">
       <c r="A26" s="1">
         <v>24</v>
       </c>
@@ -1609,7 +1609,7 @@
         <v>220</v>
       </c>
     </row>
-    <row r="27" spans="1:4" x14ac:dyDescent="0.2">
+    <row r="27" spans="1:4" x14ac:dyDescent="0.3">
       <c r="A27" s="1">
         <v>25</v>
       </c>
@@ -1623,7 +1623,7 @@
         <v>224</v>
       </c>
     </row>
-    <row r="28" spans="1:4" x14ac:dyDescent="0.2">
+    <row r="28" spans="1:4" x14ac:dyDescent="0.3">
       <c r="A28" s="1">
         <v>26</v>
       </c>
@@ -1637,7 +1637,7 @@
         <v>221</v>
       </c>
     </row>
-    <row r="29" spans="1:4" x14ac:dyDescent="0.2">
+    <row r="29" spans="1:4" x14ac:dyDescent="0.3">
       <c r="A29" s="1">
         <v>27</v>
       </c>
@@ -1651,7 +1651,7 @@
         <v>221</v>
       </c>
     </row>
-    <row r="30" spans="1:4" x14ac:dyDescent="0.2">
+    <row r="30" spans="1:4" x14ac:dyDescent="0.3">
       <c r="A30" s="1">
         <v>28</v>
       </c>
@@ -1665,7 +1665,7 @@
         <v>221</v>
       </c>
     </row>
-    <row r="31" spans="1:4" x14ac:dyDescent="0.2">
+    <row r="31" spans="1:4" x14ac:dyDescent="0.3">
       <c r="A31" s="1">
         <v>29</v>
       </c>
@@ -1679,7 +1679,7 @@
         <v>221</v>
       </c>
     </row>
-    <row r="32" spans="1:4" x14ac:dyDescent="0.2">
+    <row r="32" spans="1:4" x14ac:dyDescent="0.3">
       <c r="A32" s="1">
         <v>30</v>
       </c>
@@ -1693,7 +1693,7 @@
         <v>221</v>
       </c>
     </row>
-    <row r="33" spans="1:4" x14ac:dyDescent="0.2">
+    <row r="33" spans="1:4" x14ac:dyDescent="0.3">
       <c r="A33" s="1">
         <v>31</v>
       </c>
@@ -1707,7 +1707,7 @@
         <v>221</v>
       </c>
     </row>
-    <row r="34" spans="1:4" x14ac:dyDescent="0.2">
+    <row r="34" spans="1:4" x14ac:dyDescent="0.3">
       <c r="A34" s="1">
         <v>32</v>
       </c>
@@ -1721,7 +1721,7 @@
         <v>221</v>
       </c>
     </row>
-    <row r="35" spans="1:4" x14ac:dyDescent="0.2">
+    <row r="35" spans="1:4" x14ac:dyDescent="0.3">
       <c r="A35" s="1">
         <v>33</v>
       </c>
@@ -1735,7 +1735,7 @@
         <v>221</v>
       </c>
     </row>
-    <row r="36" spans="1:4" x14ac:dyDescent="0.2">
+    <row r="36" spans="1:4" x14ac:dyDescent="0.3">
       <c r="A36" s="1">
         <v>34</v>
       </c>
@@ -1749,7 +1749,7 @@
         <v>221</v>
       </c>
     </row>
-    <row r="37" spans="1:4" x14ac:dyDescent="0.2">
+    <row r="37" spans="1:4" x14ac:dyDescent="0.3">
       <c r="A37" s="1">
         <v>35</v>
       </c>
@@ -1763,7 +1763,7 @@
         <v>222</v>
       </c>
     </row>
-    <row r="38" spans="1:4" x14ac:dyDescent="0.2">
+    <row r="38" spans="1:4" x14ac:dyDescent="0.3">
       <c r="A38" s="1">
         <v>36</v>
       </c>
@@ -1777,7 +1777,7 @@
         <v>221</v>
       </c>
     </row>
-    <row r="39" spans="1:4" x14ac:dyDescent="0.2">
+    <row r="39" spans="1:4" x14ac:dyDescent="0.3">
       <c r="A39" s="1">
         <v>37</v>
       </c>
@@ -1791,7 +1791,7 @@
         <v>220</v>
       </c>
     </row>
-    <row r="40" spans="1:4" x14ac:dyDescent="0.2">
+    <row r="40" spans="1:4" x14ac:dyDescent="0.3">
       <c r="A40" s="1">
         <v>38</v>
       </c>
@@ -1805,7 +1805,7 @@
         <v>223</v>
       </c>
     </row>
-    <row r="41" spans="1:4" x14ac:dyDescent="0.2">
+    <row r="41" spans="1:4" x14ac:dyDescent="0.3">
       <c r="A41" s="1">
         <v>39</v>
       </c>
@@ -1819,7 +1819,7 @@
         <v>221</v>
       </c>
     </row>
-    <row r="42" spans="1:4" x14ac:dyDescent="0.2">
+    <row r="42" spans="1:4" x14ac:dyDescent="0.3">
       <c r="A42" s="1">
         <v>40</v>
       </c>
@@ -1833,7 +1833,7 @@
         <v>221</v>
       </c>
     </row>
-    <row r="43" spans="1:4" x14ac:dyDescent="0.2">
+    <row r="43" spans="1:4" x14ac:dyDescent="0.3">
       <c r="A43" s="1">
         <v>41</v>
       </c>
@@ -1847,7 +1847,7 @@
         <v>221</v>
       </c>
     </row>
-    <row r="44" spans="1:4" x14ac:dyDescent="0.2">
+    <row r="44" spans="1:4" x14ac:dyDescent="0.3">
       <c r="A44" s="1">
         <v>42</v>
       </c>
@@ -1861,7 +1861,7 @@
         <v>221</v>
       </c>
     </row>
-    <row r="45" spans="1:4" x14ac:dyDescent="0.2">
+    <row r="45" spans="1:4" x14ac:dyDescent="0.3">
       <c r="A45" s="1">
         <v>43</v>
       </c>
@@ -1875,7 +1875,7 @@
         <v>221</v>
       </c>
     </row>
-    <row r="46" spans="1:4" x14ac:dyDescent="0.2">
+    <row r="46" spans="1:4" x14ac:dyDescent="0.3">
       <c r="A46" s="1">
         <v>44</v>
       </c>
@@ -1889,7 +1889,7 @@
         <v>221</v>
       </c>
     </row>
-    <row r="47" spans="1:4" x14ac:dyDescent="0.2">
+    <row r="47" spans="1:4" x14ac:dyDescent="0.3">
       <c r="A47" s="1">
         <v>45</v>
       </c>
@@ -1903,7 +1903,7 @@
         <v>221</v>
       </c>
     </row>
-    <row r="48" spans="1:4" x14ac:dyDescent="0.2">
+    <row r="48" spans="1:4" x14ac:dyDescent="0.3">
       <c r="A48" s="1">
         <v>46</v>
       </c>
@@ -1917,7 +1917,7 @@
         <v>221</v>
       </c>
     </row>
-    <row r="49" spans="1:4" x14ac:dyDescent="0.2">
+    <row r="49" spans="1:4" x14ac:dyDescent="0.3">
       <c r="A49" s="1">
         <v>47</v>
       </c>
@@ -1931,7 +1931,7 @@
         <v>222</v>
       </c>
     </row>
-    <row r="50" spans="1:4" x14ac:dyDescent="0.2">
+    <row r="50" spans="1:4" x14ac:dyDescent="0.3">
       <c r="A50" s="1">
         <v>48</v>
       </c>
@@ -1945,7 +1945,7 @@
         <v>220</v>
       </c>
     </row>
-    <row r="51" spans="1:4" x14ac:dyDescent="0.2">
+    <row r="51" spans="1:4" x14ac:dyDescent="0.3">
       <c r="A51" s="1">
         <v>49</v>
       </c>
@@ -1959,7 +1959,7 @@
         <v>220</v>
       </c>
     </row>
-    <row r="52" spans="1:4" x14ac:dyDescent="0.2">
+    <row r="52" spans="1:4" x14ac:dyDescent="0.3">
       <c r="A52" s="1">
         <v>50</v>
       </c>
@@ -1973,7 +1973,7 @@
         <v>224</v>
       </c>
     </row>
-    <row r="53" spans="1:4" x14ac:dyDescent="0.2">
+    <row r="53" spans="1:4" x14ac:dyDescent="0.3">
       <c r="A53" s="1">
         <v>51</v>
       </c>
@@ -1987,7 +1987,7 @@
         <v>221</v>
       </c>
     </row>
-    <row r="54" spans="1:4" x14ac:dyDescent="0.2">
+    <row r="54" spans="1:4" x14ac:dyDescent="0.3">
       <c r="A54" s="1">
         <v>52</v>
       </c>
@@ -2001,7 +2001,7 @@
         <v>221</v>
       </c>
     </row>
-    <row r="55" spans="1:4" x14ac:dyDescent="0.2">
+    <row r="55" spans="1:4" x14ac:dyDescent="0.3">
       <c r="A55" s="1">
         <v>53</v>
       </c>
@@ -2015,7 +2015,7 @@
         <v>221</v>
       </c>
     </row>
-    <row r="56" spans="1:4" x14ac:dyDescent="0.2">
+    <row r="56" spans="1:4" x14ac:dyDescent="0.3">
       <c r="A56" s="1">
         <v>54</v>
       </c>
@@ -2029,7 +2029,7 @@
         <v>221</v>
       </c>
     </row>
-    <row r="57" spans="1:4" x14ac:dyDescent="0.2">
+    <row r="57" spans="1:4" x14ac:dyDescent="0.3">
       <c r="A57" s="1">
         <v>55</v>
       </c>
@@ -2043,7 +2043,7 @@
         <v>221</v>
       </c>
     </row>
-    <row r="58" spans="1:4" x14ac:dyDescent="0.2">
+    <row r="58" spans="1:4" x14ac:dyDescent="0.3">
       <c r="A58" s="1">
         <v>56</v>
       </c>
@@ -2057,7 +2057,7 @@
         <v>221</v>
       </c>
     </row>
-    <row r="59" spans="1:4" x14ac:dyDescent="0.2">
+    <row r="59" spans="1:4" x14ac:dyDescent="0.3">
       <c r="A59" s="1">
         <v>57</v>
       </c>
@@ -2071,7 +2071,7 @@
         <v>221</v>
       </c>
     </row>
-    <row r="60" spans="1:4" x14ac:dyDescent="0.2">
+    <row r="60" spans="1:4" x14ac:dyDescent="0.3">
       <c r="A60" s="1">
         <v>58</v>
       </c>
@@ -2085,7 +2085,7 @@
         <v>221</v>
       </c>
     </row>
-    <row r="61" spans="1:4" x14ac:dyDescent="0.2">
+    <row r="61" spans="1:4" x14ac:dyDescent="0.3">
       <c r="A61" s="1">
         <v>59</v>
       </c>
@@ -2099,7 +2099,7 @@
         <v>222</v>
       </c>
     </row>
-    <row r="62" spans="1:4" x14ac:dyDescent="0.2">
+    <row r="62" spans="1:4" x14ac:dyDescent="0.3">
       <c r="A62" s="1">
         <v>60</v>
       </c>
@@ -2113,7 +2113,7 @@
         <v>220</v>
       </c>
     </row>
-    <row r="63" spans="1:4" x14ac:dyDescent="0.2">
+    <row r="63" spans="1:4" x14ac:dyDescent="0.3">
       <c r="A63" s="1">
         <v>61</v>
       </c>
@@ -2127,7 +2127,7 @@
         <v>220</v>
       </c>
     </row>
-    <row r="64" spans="1:4" x14ac:dyDescent="0.2">
+    <row r="64" spans="1:4" x14ac:dyDescent="0.3">
       <c r="A64" s="1">
         <v>62</v>
       </c>
@@ -2141,7 +2141,7 @@
         <v>220</v>
       </c>
     </row>
-    <row r="65" spans="1:4" x14ac:dyDescent="0.2">
+    <row r="65" spans="1:4" x14ac:dyDescent="0.3">
       <c r="A65" s="1">
         <v>63</v>
       </c>
@@ -2155,7 +2155,7 @@
         <v>224</v>
       </c>
     </row>
-    <row r="66" spans="1:4" x14ac:dyDescent="0.2">
+    <row r="66" spans="1:4" x14ac:dyDescent="0.3">
       <c r="A66" s="1">
         <v>64</v>
       </c>
@@ -2169,7 +2169,7 @@
         <v>221</v>
       </c>
     </row>
-    <row r="67" spans="1:4" x14ac:dyDescent="0.2">
+    <row r="67" spans="1:4" x14ac:dyDescent="0.3">
       <c r="A67" s="1">
         <v>65</v>
       </c>
@@ -2183,7 +2183,7 @@
         <v>221</v>
       </c>
     </row>
-    <row r="68" spans="1:4" x14ac:dyDescent="0.2">
+    <row r="68" spans="1:4" x14ac:dyDescent="0.3">
       <c r="A68" s="1">
         <v>66</v>
       </c>
@@ -2197,7 +2197,7 @@
         <v>221</v>
       </c>
     </row>
-    <row r="69" spans="1:4" x14ac:dyDescent="0.2">
+    <row r="69" spans="1:4" x14ac:dyDescent="0.3">
       <c r="A69" s="1">
         <v>67</v>
       </c>
@@ -2211,7 +2211,7 @@
         <v>221</v>
       </c>
     </row>
-    <row r="70" spans="1:4" x14ac:dyDescent="0.2">
+    <row r="70" spans="1:4" x14ac:dyDescent="0.3">
       <c r="A70" s="1">
         <v>68</v>
       </c>
@@ -2225,7 +2225,7 @@
         <v>221</v>
       </c>
     </row>
-    <row r="71" spans="1:4" x14ac:dyDescent="0.2">
+    <row r="71" spans="1:4" x14ac:dyDescent="0.3">
       <c r="A71" s="1">
         <v>69</v>
       </c>
@@ -2239,7 +2239,7 @@
         <v>221</v>
       </c>
     </row>
-    <row r="72" spans="1:4" x14ac:dyDescent="0.2">
+    <row r="72" spans="1:4" x14ac:dyDescent="0.3">
       <c r="A72" s="1">
         <v>70</v>
       </c>
@@ -2253,7 +2253,7 @@
         <v>221</v>
       </c>
     </row>
-    <row r="73" spans="1:4" x14ac:dyDescent="0.2">
+    <row r="73" spans="1:4" x14ac:dyDescent="0.3">
       <c r="A73" s="1">
         <v>71</v>
       </c>
@@ -2267,7 +2267,7 @@
         <v>222</v>
       </c>
     </row>
-    <row r="74" spans="1:4" x14ac:dyDescent="0.2">
+    <row r="74" spans="1:4" x14ac:dyDescent="0.3">
       <c r="A74" s="1">
         <v>72</v>
       </c>
@@ -2281,7 +2281,7 @@
         <v>220</v>
       </c>
     </row>
-    <row r="75" spans="1:4" x14ac:dyDescent="0.2">
+    <row r="75" spans="1:4" x14ac:dyDescent="0.3">
       <c r="A75" s="1">
         <v>73</v>
       </c>
@@ -2295,7 +2295,7 @@
         <v>220</v>
       </c>
     </row>
-    <row r="76" spans="1:4" x14ac:dyDescent="0.2">
+    <row r="76" spans="1:4" x14ac:dyDescent="0.3">
       <c r="A76" s="1">
         <v>74</v>
       </c>
@@ -2309,7 +2309,7 @@
         <v>223</v>
       </c>
     </row>
-    <row r="77" spans="1:4" x14ac:dyDescent="0.2">
+    <row r="77" spans="1:4" x14ac:dyDescent="0.3">
       <c r="A77" s="1">
         <v>75</v>
       </c>
@@ -2323,7 +2323,7 @@
         <v>221</v>
       </c>
     </row>
-    <row r="78" spans="1:4" x14ac:dyDescent="0.2">
+    <row r="78" spans="1:4" x14ac:dyDescent="0.3">
       <c r="A78" s="1">
         <v>76</v>
       </c>
@@ -2337,7 +2337,7 @@
         <v>221</v>
       </c>
     </row>
-    <row r="79" spans="1:4" x14ac:dyDescent="0.2">
+    <row r="79" spans="1:4" x14ac:dyDescent="0.3">
       <c r="A79" s="1">
         <v>77</v>
       </c>
@@ -2351,7 +2351,7 @@
         <v>221</v>
       </c>
     </row>
-    <row r="80" spans="1:4" x14ac:dyDescent="0.2">
+    <row r="80" spans="1:4" x14ac:dyDescent="0.3">
       <c r="A80" s="1">
         <v>78</v>
       </c>
@@ -2365,7 +2365,7 @@
         <v>221</v>
       </c>
     </row>
-    <row r="81" spans="1:4" x14ac:dyDescent="0.2">
+    <row r="81" spans="1:4" x14ac:dyDescent="0.3">
       <c r="A81" s="1">
         <v>79</v>
       </c>
@@ -2379,7 +2379,7 @@
         <v>221</v>
       </c>
     </row>
-    <row r="82" spans="1:4" x14ac:dyDescent="0.2">
+    <row r="82" spans="1:4" x14ac:dyDescent="0.3">
       <c r="A82" s="1">
         <v>80</v>
       </c>
@@ -2393,7 +2393,7 @@
         <v>221</v>
       </c>
     </row>
-    <row r="83" spans="1:4" x14ac:dyDescent="0.2">
+    <row r="83" spans="1:4" x14ac:dyDescent="0.3">
       <c r="A83" s="1">
         <v>81</v>
       </c>
@@ -2407,7 +2407,7 @@
         <v>222</v>
       </c>
     </row>
-    <row r="84" spans="1:4" x14ac:dyDescent="0.2">
+    <row r="84" spans="1:4" x14ac:dyDescent="0.3">
       <c r="A84" s="1">
         <v>82</v>
       </c>
@@ -2421,7 +2421,7 @@
         <v>222</v>
       </c>
     </row>
-    <row r="85" spans="1:4" x14ac:dyDescent="0.2">
+    <row r="85" spans="1:4" x14ac:dyDescent="0.3">
       <c r="A85" s="1">
         <v>83</v>
       </c>
@@ -2435,7 +2435,7 @@
         <v>221</v>
       </c>
     </row>
-    <row r="86" spans="1:4" x14ac:dyDescent="0.2">
+    <row r="86" spans="1:4" x14ac:dyDescent="0.3">
       <c r="A86" s="1">
         <v>84</v>
       </c>
@@ -2449,7 +2449,7 @@
         <v>220</v>
       </c>
     </row>
-    <row r="87" spans="1:4" x14ac:dyDescent="0.2">
+    <row r="87" spans="1:4" x14ac:dyDescent="0.3">
       <c r="A87" s="1">
         <v>85</v>
       </c>
@@ -2463,7 +2463,7 @@
         <v>221</v>
       </c>
     </row>
-    <row r="88" spans="1:4" x14ac:dyDescent="0.2">
+    <row r="88" spans="1:4" x14ac:dyDescent="0.3">
       <c r="A88" s="1">
         <v>86</v>
       </c>
@@ -2477,7 +2477,7 @@
         <v>224</v>
       </c>
     </row>
-    <row r="89" spans="1:4" x14ac:dyDescent="0.2">
+    <row r="89" spans="1:4" x14ac:dyDescent="0.3">
       <c r="A89" s="1">
         <v>87</v>
       </c>
@@ -2491,7 +2491,7 @@
         <v>224</v>
       </c>
     </row>
-    <row r="90" spans="1:4" x14ac:dyDescent="0.2">
+    <row r="90" spans="1:4" x14ac:dyDescent="0.3">
       <c r="A90" s="1">
         <v>88</v>
       </c>
@@ -2505,7 +2505,7 @@
         <v>220</v>
       </c>
     </row>
-    <row r="91" spans="1:4" x14ac:dyDescent="0.2">
+    <row r="91" spans="1:4" x14ac:dyDescent="0.3">
       <c r="A91" s="1">
         <v>89</v>
       </c>
@@ -2519,7 +2519,7 @@
         <v>220</v>
       </c>
     </row>
-    <row r="92" spans="1:4" x14ac:dyDescent="0.2">
+    <row r="92" spans="1:4" x14ac:dyDescent="0.3">
       <c r="A92" s="1">
         <v>90</v>
       </c>
@@ -2533,7 +2533,7 @@
         <v>222</v>
       </c>
     </row>
-    <row r="93" spans="1:4" x14ac:dyDescent="0.2">
+    <row r="93" spans="1:4" x14ac:dyDescent="0.3">
       <c r="A93" s="1">
         <v>91</v>
       </c>
@@ -2547,7 +2547,7 @@
         <v>220</v>
       </c>
     </row>
-    <row r="94" spans="1:4" x14ac:dyDescent="0.2">
+    <row r="94" spans="1:4" x14ac:dyDescent="0.3">
       <c r="A94" s="1">
         <v>92</v>
       </c>
@@ -2561,7 +2561,7 @@
         <v>221</v>
       </c>
     </row>
-    <row r="95" spans="1:4" x14ac:dyDescent="0.2">
+    <row r="95" spans="1:4" x14ac:dyDescent="0.3">
       <c r="A95" s="1">
         <v>93</v>
       </c>
@@ -2575,7 +2575,7 @@
         <v>221</v>
       </c>
     </row>
-    <row r="96" spans="1:4" x14ac:dyDescent="0.2">
+    <row r="96" spans="1:4" x14ac:dyDescent="0.3">
       <c r="A96" s="1">
         <v>94</v>
       </c>
@@ -2589,7 +2589,7 @@
         <v>223</v>
       </c>
     </row>
-    <row r="97" spans="1:4" x14ac:dyDescent="0.2">
+    <row r="97" spans="1:4" x14ac:dyDescent="0.3">
       <c r="A97" s="1">
         <v>95</v>
       </c>
@@ -2603,7 +2603,7 @@
         <v>220</v>
       </c>
     </row>
-    <row r="98" spans="1:4" x14ac:dyDescent="0.2">
+    <row r="98" spans="1:4" x14ac:dyDescent="0.3">
       <c r="A98" s="1">
         <v>96</v>
       </c>
@@ -2617,7 +2617,7 @@
         <v>221</v>
       </c>
     </row>
-    <row r="99" spans="1:4" x14ac:dyDescent="0.2">
+    <row r="99" spans="1:4" x14ac:dyDescent="0.3">
       <c r="A99" s="1">
         <v>97</v>
       </c>
@@ -2631,7 +2631,7 @@
         <v>221</v>
       </c>
     </row>
-    <row r="100" spans="1:4" x14ac:dyDescent="0.2">
+    <row r="100" spans="1:4" x14ac:dyDescent="0.3">
       <c r="A100" s="1">
         <v>98</v>
       </c>
@@ -2645,7 +2645,7 @@
         <v>221</v>
       </c>
     </row>
-    <row r="101" spans="1:4" x14ac:dyDescent="0.2">
+    <row r="101" spans="1:4" x14ac:dyDescent="0.3">
       <c r="A101" s="1">
         <v>99</v>
       </c>
@@ -2659,7 +2659,7 @@
         <v>223</v>
       </c>
     </row>
-    <row r="102" spans="1:4" x14ac:dyDescent="0.2">
+    <row r="102" spans="1:4" x14ac:dyDescent="0.3">
       <c r="A102" s="1">
         <v>100</v>
       </c>
@@ -2673,7 +2673,7 @@
         <v>223</v>
       </c>
     </row>
-    <row r="103" spans="1:4" x14ac:dyDescent="0.2">
+    <row r="103" spans="1:4" x14ac:dyDescent="0.3">
       <c r="A103" s="1">
         <v>101</v>
       </c>
@@ -2687,7 +2687,7 @@
         <v>222</v>
       </c>
     </row>
-    <row r="104" spans="1:4" x14ac:dyDescent="0.2">
+    <row r="104" spans="1:4" x14ac:dyDescent="0.3">
       <c r="A104" s="1">
         <v>102</v>
       </c>
@@ -2701,7 +2701,7 @@
         <v>220</v>
       </c>
     </row>
-    <row r="105" spans="1:4" x14ac:dyDescent="0.2">
+    <row r="105" spans="1:4" x14ac:dyDescent="0.3">
       <c r="A105" s="1">
         <v>103</v>
       </c>
@@ -2715,7 +2715,7 @@
         <v>223</v>
       </c>
     </row>
-    <row r="106" spans="1:4" x14ac:dyDescent="0.2">
+    <row r="106" spans="1:4" x14ac:dyDescent="0.3">
       <c r="A106" s="1">
         <v>104</v>
       </c>
@@ -2729,7 +2729,7 @@
         <v>221</v>
       </c>
     </row>
-    <row r="107" spans="1:4" x14ac:dyDescent="0.2">
+    <row r="107" spans="1:4" x14ac:dyDescent="0.3">
       <c r="A107" s="1">
         <v>105</v>
       </c>
@@ -2743,7 +2743,7 @@
         <v>221</v>
       </c>
     </row>
-    <row r="108" spans="1:4" x14ac:dyDescent="0.2">
+    <row r="108" spans="1:4" x14ac:dyDescent="0.3">
       <c r="A108" s="1">
         <v>106</v>
       </c>
@@ -2757,7 +2757,7 @@
         <v>221</v>
       </c>
     </row>
-    <row r="109" spans="1:4" x14ac:dyDescent="0.2">
+    <row r="109" spans="1:4" x14ac:dyDescent="0.3">
       <c r="A109" s="1">
         <v>107</v>
       </c>
@@ -2771,7 +2771,7 @@
         <v>222</v>
       </c>
     </row>
-    <row r="110" spans="1:4" x14ac:dyDescent="0.2">
+    <row r="110" spans="1:4" x14ac:dyDescent="0.3">
       <c r="A110" s="1">
         <v>108</v>
       </c>
@@ -2785,7 +2785,7 @@
         <v>220</v>
       </c>
     </row>
-    <row r="111" spans="1:4" x14ac:dyDescent="0.2">
+    <row r="111" spans="1:4" x14ac:dyDescent="0.3">
       <c r="A111" s="1">
         <v>109</v>
       </c>
@@ -2799,7 +2799,7 @@
         <v>220</v>
       </c>
     </row>
-    <row r="112" spans="1:4" x14ac:dyDescent="0.2">
+    <row r="112" spans="1:4" x14ac:dyDescent="0.3">
       <c r="A112" s="1">
         <v>110</v>
       </c>
@@ -2813,7 +2813,7 @@
         <v>223</v>
       </c>
     </row>
-    <row r="113" spans="1:4" x14ac:dyDescent="0.2">
+    <row r="113" spans="1:4" x14ac:dyDescent="0.3">
       <c r="A113" s="1">
         <v>111</v>
       </c>
@@ -2827,7 +2827,7 @@
         <v>223</v>
       </c>
     </row>
-    <row r="114" spans="1:4" x14ac:dyDescent="0.2">
+    <row r="114" spans="1:4" x14ac:dyDescent="0.3">
       <c r="A114" s="1">
         <v>112</v>
       </c>
@@ -2841,7 +2841,7 @@
         <v>221</v>
       </c>
     </row>
-    <row r="115" spans="1:4" x14ac:dyDescent="0.2">
+    <row r="115" spans="1:4" x14ac:dyDescent="0.3">
       <c r="A115" s="1">
         <v>113</v>
       </c>
@@ -2855,7 +2855,7 @@
         <v>221</v>
       </c>
     </row>
-    <row r="116" spans="1:4" x14ac:dyDescent="0.2">
+    <row r="116" spans="1:4" x14ac:dyDescent="0.3">
       <c r="A116" s="1">
         <v>114</v>
       </c>
@@ -2869,7 +2869,7 @@
         <v>221</v>
       </c>
     </row>
-    <row r="117" spans="1:4" x14ac:dyDescent="0.2">
+    <row r="117" spans="1:4" x14ac:dyDescent="0.3">
       <c r="A117" s="1">
         <v>115</v>
       </c>
@@ -2883,7 +2883,7 @@
         <v>221</v>
       </c>
     </row>
-    <row r="118" spans="1:4" x14ac:dyDescent="0.2">
+    <row r="118" spans="1:4" x14ac:dyDescent="0.3">
       <c r="A118" s="1">
         <v>116</v>
       </c>
@@ -2897,7 +2897,7 @@
         <v>221</v>
       </c>
     </row>
-    <row r="119" spans="1:4" x14ac:dyDescent="0.2">
+    <row r="119" spans="1:4" x14ac:dyDescent="0.3">
       <c r="A119" s="1">
         <v>117</v>
       </c>
@@ -2911,7 +2911,7 @@
         <v>221</v>
       </c>
     </row>
-    <row r="120" spans="1:4" x14ac:dyDescent="0.2">
+    <row r="120" spans="1:4" x14ac:dyDescent="0.3">
       <c r="A120" s="1">
         <v>118</v>
       </c>
@@ -2925,7 +2925,7 @@
         <v>221</v>
       </c>
     </row>
-    <row r="121" spans="1:4" x14ac:dyDescent="0.2">
+    <row r="121" spans="1:4" x14ac:dyDescent="0.3">
       <c r="A121" s="1">
         <v>119</v>
       </c>
@@ -2939,7 +2939,7 @@
         <v>223</v>
       </c>
     </row>
-    <row r="122" spans="1:4" x14ac:dyDescent="0.2">
+    <row r="122" spans="1:4" x14ac:dyDescent="0.3">
       <c r="A122" s="1">
         <v>120</v>
       </c>
@@ -2953,7 +2953,7 @@
         <v>220</v>
       </c>
     </row>
-    <row r="123" spans="1:4" x14ac:dyDescent="0.2">
+    <row r="123" spans="1:4" x14ac:dyDescent="0.3">
       <c r="A123" s="1">
         <v>121</v>
       </c>
@@ -2967,7 +2967,7 @@
         <v>222</v>
       </c>
     </row>
-    <row r="124" spans="1:4" x14ac:dyDescent="0.2">
+    <row r="124" spans="1:4" x14ac:dyDescent="0.3">
       <c r="A124" s="1">
         <v>122</v>
       </c>
@@ -2981,7 +2981,7 @@
         <v>220</v>
       </c>
     </row>
-    <row r="125" spans="1:4" x14ac:dyDescent="0.2">
+    <row r="125" spans="1:4" x14ac:dyDescent="0.3">
       <c r="A125" s="1">
         <v>123</v>
       </c>
@@ -2995,7 +2995,7 @@
         <v>220</v>
       </c>
     </row>
-    <row r="126" spans="1:4" x14ac:dyDescent="0.2">
+    <row r="126" spans="1:4" x14ac:dyDescent="0.3">
       <c r="A126" s="1">
         <v>124</v>
       </c>
@@ -3009,7 +3009,7 @@
         <v>223</v>
       </c>
     </row>
-    <row r="127" spans="1:4" x14ac:dyDescent="0.2">
+    <row r="127" spans="1:4" x14ac:dyDescent="0.3">
       <c r="A127" s="1">
         <v>125</v>
       </c>
@@ -3023,7 +3023,7 @@
         <v>223</v>
       </c>
     </row>
-    <row r="128" spans="1:4" x14ac:dyDescent="0.2">
+    <row r="128" spans="1:4" x14ac:dyDescent="0.3">
       <c r="A128" s="1">
         <v>126</v>
       </c>
@@ -3037,7 +3037,7 @@
         <v>221</v>
       </c>
     </row>
-    <row r="129" spans="1:4" x14ac:dyDescent="0.2">
+    <row r="129" spans="1:4" x14ac:dyDescent="0.3">
       <c r="A129" s="1">
         <v>127</v>
       </c>
@@ -3051,7 +3051,7 @@
         <v>221</v>
       </c>
     </row>
-    <row r="130" spans="1:4" x14ac:dyDescent="0.2">
+    <row r="130" spans="1:4" x14ac:dyDescent="0.3">
       <c r="A130" s="1">
         <v>128</v>
       </c>
@@ -3065,7 +3065,7 @@
         <v>221</v>
       </c>
     </row>
-    <row r="131" spans="1:4" x14ac:dyDescent="0.2">
+    <row r="131" spans="1:4" x14ac:dyDescent="0.3">
       <c r="A131" s="1">
         <v>129</v>
       </c>
@@ -3079,7 +3079,7 @@
         <v>221</v>
       </c>
     </row>
-    <row r="132" spans="1:4" x14ac:dyDescent="0.2">
+    <row r="132" spans="1:4" x14ac:dyDescent="0.3">
       <c r="A132" s="1">
         <v>130</v>
       </c>
@@ -3093,7 +3093,7 @@
         <v>221</v>
       </c>
     </row>
-    <row r="133" spans="1:4" x14ac:dyDescent="0.2">
+    <row r="133" spans="1:4" x14ac:dyDescent="0.3">
       <c r="A133" s="1">
         <v>131</v>
       </c>
@@ -3107,7 +3107,7 @@
         <v>221</v>
       </c>
     </row>
-    <row r="134" spans="1:4" x14ac:dyDescent="0.2">
+    <row r="134" spans="1:4" x14ac:dyDescent="0.3">
       <c r="A134" s="1">
         <v>132</v>
       </c>
@@ -3121,7 +3121,7 @@
         <v>221</v>
       </c>
     </row>
-    <row r="135" spans="1:4" x14ac:dyDescent="0.2">
+    <row r="135" spans="1:4" x14ac:dyDescent="0.3">
       <c r="A135" s="1">
         <v>133</v>
       </c>
@@ -3135,7 +3135,7 @@
         <v>221</v>
       </c>
     </row>
-    <row r="136" spans="1:4" x14ac:dyDescent="0.2">
+    <row r="136" spans="1:4" x14ac:dyDescent="0.3">
       <c r="A136" s="1">
         <v>134</v>
       </c>
@@ -3149,7 +3149,7 @@
         <v>220</v>
       </c>
     </row>
-    <row r="137" spans="1:4" x14ac:dyDescent="0.2">
+    <row r="137" spans="1:4" x14ac:dyDescent="0.3">
       <c r="A137" s="1">
         <v>135</v>
       </c>
@@ -3163,7 +3163,7 @@
         <v>221</v>
       </c>
     </row>
-    <row r="138" spans="1:4" x14ac:dyDescent="0.2">
+    <row r="138" spans="1:4" x14ac:dyDescent="0.3">
       <c r="A138" s="1">
         <v>136</v>
       </c>
@@ -3177,7 +3177,7 @@
         <v>221</v>
       </c>
     </row>
-    <row r="139" spans="1:4" x14ac:dyDescent="0.2">
+    <row r="139" spans="1:4" x14ac:dyDescent="0.3">
       <c r="A139" s="1">
         <v>137</v>
       </c>
@@ -3191,7 +3191,7 @@
         <v>221</v>
       </c>
     </row>
-    <row r="140" spans="1:4" x14ac:dyDescent="0.2">
+    <row r="140" spans="1:4" x14ac:dyDescent="0.3">
       <c r="A140" s="1">
         <v>138</v>
       </c>
@@ -3205,7 +3205,7 @@
         <v>221</v>
       </c>
     </row>
-    <row r="141" spans="1:4" x14ac:dyDescent="0.2">
+    <row r="141" spans="1:4" x14ac:dyDescent="0.3">
       <c r="A141" s="1">
         <v>139</v>
       </c>
@@ -3219,7 +3219,7 @@
         <v>221</v>
       </c>
     </row>
-    <row r="142" spans="1:4" x14ac:dyDescent="0.2">
+    <row r="142" spans="1:4" x14ac:dyDescent="0.3">
       <c r="A142" s="1">
         <v>140</v>
       </c>
@@ -3233,7 +3233,7 @@
         <v>221</v>
       </c>
     </row>
-    <row r="143" spans="1:4" x14ac:dyDescent="0.2">
+    <row r="143" spans="1:4" x14ac:dyDescent="0.3">
       <c r="A143" s="1">
         <v>141</v>
       </c>
@@ -3247,7 +3247,7 @@
         <v>222</v>
       </c>
     </row>
-    <row r="144" spans="1:4" x14ac:dyDescent="0.2">
+    <row r="144" spans="1:4" x14ac:dyDescent="0.3">
       <c r="A144" s="1">
         <v>142</v>
       </c>
@@ -3261,7 +3261,7 @@
         <v>223</v>
       </c>
     </row>
-    <row r="145" spans="1:4" x14ac:dyDescent="0.2">
+    <row r="145" spans="1:4" x14ac:dyDescent="0.3">
       <c r="A145" s="1">
         <v>143</v>
       </c>
@@ -3275,7 +3275,7 @@
         <v>221</v>
       </c>
     </row>
-    <row r="146" spans="1:4" x14ac:dyDescent="0.2">
+    <row r="146" spans="1:4" x14ac:dyDescent="0.3">
       <c r="A146" s="1">
         <v>144</v>
       </c>
@@ -3289,7 +3289,7 @@
         <v>222</v>
       </c>
     </row>
-    <row r="147" spans="1:4" x14ac:dyDescent="0.2">
+    <row r="147" spans="1:4" x14ac:dyDescent="0.3">
       <c r="A147" s="1">
         <v>145</v>
       </c>
@@ -3303,7 +3303,7 @@
         <v>220</v>
       </c>
     </row>
-    <row r="148" spans="1:4" x14ac:dyDescent="0.2">
+    <row r="148" spans="1:4" x14ac:dyDescent="0.3">
       <c r="A148" s="1">
         <v>146</v>
       </c>
@@ -3317,7 +3317,7 @@
         <v>220</v>
       </c>
     </row>
-    <row r="149" spans="1:4" x14ac:dyDescent="0.2">
+    <row r="149" spans="1:4" x14ac:dyDescent="0.3">
       <c r="A149" s="1">
         <v>147</v>
       </c>
@@ -3331,7 +3331,7 @@
         <v>224</v>
       </c>
     </row>
-    <row r="150" spans="1:4" x14ac:dyDescent="0.2">
+    <row r="150" spans="1:4" x14ac:dyDescent="0.3">
       <c r="A150" s="1">
         <v>148</v>
       </c>
@@ -3345,7 +3345,7 @@
         <v>224</v>
       </c>
     </row>
-    <row r="151" spans="1:4" x14ac:dyDescent="0.2">
+    <row r="151" spans="1:4" x14ac:dyDescent="0.3">
       <c r="A151" s="1">
         <v>149</v>
       </c>
@@ -3359,7 +3359,7 @@
         <v>224</v>
       </c>
     </row>
-    <row r="152" spans="1:4" x14ac:dyDescent="0.2">
+    <row r="152" spans="1:4" x14ac:dyDescent="0.3">
       <c r="A152" s="1">
         <v>150</v>
       </c>
@@ -3373,7 +3373,7 @@
         <v>221</v>
       </c>
     </row>
-    <row r="153" spans="1:4" x14ac:dyDescent="0.2">
+    <row r="153" spans="1:4" x14ac:dyDescent="0.3">
       <c r="A153" s="1">
         <v>151</v>
       </c>
@@ -3387,7 +3387,7 @@
         <v>221</v>
       </c>
     </row>
-    <row r="154" spans="1:4" x14ac:dyDescent="0.2">
+    <row r="154" spans="1:4" x14ac:dyDescent="0.3">
       <c r="A154" s="1">
         <v>152</v>
       </c>
@@ -3401,7 +3401,7 @@
         <v>221</v>
       </c>
     </row>
-    <row r="155" spans="1:4" x14ac:dyDescent="0.2">
+    <row r="155" spans="1:4" x14ac:dyDescent="0.3">
       <c r="A155" s="1">
         <v>153</v>
       </c>
@@ -3415,7 +3415,7 @@
         <v>221</v>
       </c>
     </row>
-    <row r="156" spans="1:4" x14ac:dyDescent="0.2">
+    <row r="156" spans="1:4" x14ac:dyDescent="0.3">
       <c r="A156" s="1">
         <v>154</v>
       </c>
@@ -3429,7 +3429,7 @@
         <v>221</v>
       </c>
     </row>
-    <row r="157" spans="1:4" x14ac:dyDescent="0.2">
+    <row r="157" spans="1:4" x14ac:dyDescent="0.3">
       <c r="A157" s="1">
         <v>155</v>
       </c>
@@ -3443,7 +3443,7 @@
         <v>221</v>
       </c>
     </row>
-    <row r="158" spans="1:4" x14ac:dyDescent="0.2">
+    <row r="158" spans="1:4" x14ac:dyDescent="0.3">
       <c r="A158" s="1">
         <v>156</v>
       </c>
@@ -3457,7 +3457,7 @@
         <v>221</v>
       </c>
     </row>
-    <row r="159" spans="1:4" x14ac:dyDescent="0.2">
+    <row r="159" spans="1:4" x14ac:dyDescent="0.3">
       <c r="A159" s="1">
         <v>157</v>
       </c>
@@ -3471,7 +3471,7 @@
         <v>221</v>
       </c>
     </row>
-    <row r="160" spans="1:4" x14ac:dyDescent="0.2">
+    <row r="160" spans="1:4" x14ac:dyDescent="0.3">
       <c r="A160" s="1">
         <v>158</v>
       </c>
@@ -3485,7 +3485,7 @@
         <v>221</v>
       </c>
     </row>
-    <row r="161" spans="1:4" x14ac:dyDescent="0.2">
+    <row r="161" spans="1:4" x14ac:dyDescent="0.3">
       <c r="A161" s="1">
         <v>159</v>
       </c>
@@ -3499,7 +3499,7 @@
         <v>221</v>
       </c>
     </row>
-    <row r="162" spans="1:4" x14ac:dyDescent="0.2">
+    <row r="162" spans="1:4" x14ac:dyDescent="0.3">
       <c r="A162" s="1">
         <v>160</v>
       </c>
@@ -3513,7 +3513,7 @@
         <v>221</v>
       </c>
     </row>
-    <row r="163" spans="1:4" x14ac:dyDescent="0.2">
+    <row r="163" spans="1:4" x14ac:dyDescent="0.3">
       <c r="A163" s="1">
         <v>161</v>
       </c>
@@ -3527,7 +3527,7 @@
         <v>221</v>
       </c>
     </row>
-    <row r="164" spans="1:4" x14ac:dyDescent="0.2">
+    <row r="164" spans="1:4" x14ac:dyDescent="0.3">
       <c r="A164" s="1">
         <v>162</v>
       </c>
@@ -3541,7 +3541,7 @@
         <v>221</v>
       </c>
     </row>
-    <row r="165" spans="1:4" x14ac:dyDescent="0.2">
+    <row r="165" spans="1:4" x14ac:dyDescent="0.3">
       <c r="A165" s="1">
         <v>163</v>
       </c>
@@ -3555,7 +3555,7 @@
         <v>221</v>
       </c>
     </row>
-    <row r="166" spans="1:4" x14ac:dyDescent="0.2">
+    <row r="166" spans="1:4" x14ac:dyDescent="0.3">
       <c r="A166" s="1">
         <v>164</v>
       </c>
@@ -3569,7 +3569,7 @@
         <v>221</v>
       </c>
     </row>
-    <row r="167" spans="1:4" x14ac:dyDescent="0.2">
+    <row r="167" spans="1:4" x14ac:dyDescent="0.3">
       <c r="A167" s="1">
         <v>165</v>
       </c>
@@ -3583,7 +3583,7 @@
         <v>221</v>
       </c>
     </row>
-    <row r="168" spans="1:4" x14ac:dyDescent="0.2">
+    <row r="168" spans="1:4" x14ac:dyDescent="0.3">
       <c r="A168" s="1">
         <v>166</v>
       </c>
@@ -3597,7 +3597,7 @@
         <v>220</v>
       </c>
     </row>
-    <row r="169" spans="1:4" x14ac:dyDescent="0.2">
+    <row r="169" spans="1:4" x14ac:dyDescent="0.3">
       <c r="A169" s="1">
         <v>167</v>
       </c>
@@ -3611,7 +3611,7 @@
         <v>224</v>
       </c>
     </row>
-    <row r="170" spans="1:4" x14ac:dyDescent="0.2">
+    <row r="170" spans="1:4" x14ac:dyDescent="0.3">
       <c r="A170" s="1">
         <v>168</v>
       </c>
@@ -3625,7 +3625,7 @@
         <v>224</v>
       </c>
     </row>
-    <row r="171" spans="1:4" x14ac:dyDescent="0.2">
+    <row r="171" spans="1:4" x14ac:dyDescent="0.3">
       <c r="A171" s="1">
         <v>169</v>
       </c>
@@ -3639,7 +3639,7 @@
         <v>224</v>
       </c>
     </row>
-    <row r="172" spans="1:4" x14ac:dyDescent="0.2">
+    <row r="172" spans="1:4" x14ac:dyDescent="0.3">
       <c r="A172" s="1">
         <v>170</v>
       </c>
@@ -3653,7 +3653,7 @@
         <v>221</v>
       </c>
     </row>
-    <row r="173" spans="1:4" x14ac:dyDescent="0.2">
+    <row r="173" spans="1:4" x14ac:dyDescent="0.3">
       <c r="A173" s="1">
         <v>171</v>
       </c>
@@ -3667,7 +3667,7 @@
         <v>221</v>
       </c>
     </row>
-    <row r="174" spans="1:4" x14ac:dyDescent="0.2">
+    <row r="174" spans="1:4" x14ac:dyDescent="0.3">
       <c r="A174" s="1">
         <v>172</v>
       </c>
@@ -3681,7 +3681,7 @@
         <v>224</v>
       </c>
     </row>
-    <row r="175" spans="1:4" x14ac:dyDescent="0.2">
+    <row r="175" spans="1:4" x14ac:dyDescent="0.3">
       <c r="A175" s="1">
         <v>173</v>
       </c>
@@ -3695,7 +3695,7 @@
         <v>222</v>
       </c>
     </row>
-    <row r="176" spans="1:4" x14ac:dyDescent="0.2">
+    <row r="176" spans="1:4" x14ac:dyDescent="0.3">
       <c r="A176" s="1">
         <v>174</v>
       </c>
@@ -3709,7 +3709,7 @@
         <v>222</v>
       </c>
     </row>
-    <row r="177" spans="1:4" x14ac:dyDescent="0.2">
+    <row r="177" spans="1:4" x14ac:dyDescent="0.3">
       <c r="A177" s="1">
         <v>175</v>
       </c>
@@ -3723,7 +3723,7 @@
         <v>220</v>
       </c>
     </row>
-    <row r="178" spans="1:4" x14ac:dyDescent="0.2">
+    <row r="178" spans="1:4" x14ac:dyDescent="0.3">
       <c r="A178" s="1">
         <v>176</v>
       </c>
@@ -3737,7 +3737,7 @@
         <v>223</v>
       </c>
     </row>
-    <row r="179" spans="1:4" x14ac:dyDescent="0.2">
+    <row r="179" spans="1:4" x14ac:dyDescent="0.3">
       <c r="A179" s="1">
         <v>177</v>
       </c>
@@ -3751,7 +3751,7 @@
         <v>223</v>
       </c>
     </row>
-    <row r="180" spans="1:4" x14ac:dyDescent="0.2">
+    <row r="180" spans="1:4" x14ac:dyDescent="0.3">
       <c r="A180" s="1">
         <v>178</v>
       </c>
@@ -3765,7 +3765,7 @@
         <v>221</v>
       </c>
     </row>
-    <row r="181" spans="1:4" x14ac:dyDescent="0.2">
+    <row r="181" spans="1:4" x14ac:dyDescent="0.3">
       <c r="A181" s="1">
         <v>179</v>
       </c>
@@ -3779,7 +3779,7 @@
         <v>221</v>
       </c>
     </row>
-    <row r="182" spans="1:4" x14ac:dyDescent="0.2">
+    <row r="182" spans="1:4" x14ac:dyDescent="0.3">
       <c r="A182" s="1">
         <v>180</v>
       </c>
@@ -3793,7 +3793,7 @@
         <v>221</v>
       </c>
     </row>
-    <row r="183" spans="1:4" x14ac:dyDescent="0.2">
+    <row r="183" spans="1:4" x14ac:dyDescent="0.3">
       <c r="A183" s="1">
         <v>181</v>
       </c>
@@ -3807,7 +3807,7 @@
         <v>221</v>
       </c>
     </row>
-    <row r="184" spans="1:4" x14ac:dyDescent="0.2">
+    <row r="184" spans="1:4" x14ac:dyDescent="0.3">
       <c r="A184" s="1">
         <v>182</v>
       </c>
@@ -3821,7 +3821,7 @@
         <v>221</v>
       </c>
     </row>
-    <row r="185" spans="1:4" x14ac:dyDescent="0.2">
+    <row r="185" spans="1:4" x14ac:dyDescent="0.3">
       <c r="A185" s="1">
         <v>183</v>
       </c>
@@ -3835,7 +3835,7 @@
         <v>222</v>
       </c>
     </row>
-    <row r="186" spans="1:4" x14ac:dyDescent="0.2">
+    <row r="186" spans="1:4" x14ac:dyDescent="0.3">
       <c r="A186" s="1">
         <v>184</v>
       </c>
@@ -3849,7 +3849,7 @@
         <v>220</v>
       </c>
     </row>
-    <row r="187" spans="1:4" x14ac:dyDescent="0.2">
+    <row r="187" spans="1:4" x14ac:dyDescent="0.3">
       <c r="A187" s="1">
         <v>185</v>
       </c>
@@ -3863,7 +3863,7 @@
         <v>223</v>
       </c>
     </row>
-    <row r="188" spans="1:4" x14ac:dyDescent="0.2">
+    <row r="188" spans="1:4" x14ac:dyDescent="0.3">
       <c r="A188" s="1">
         <v>186</v>
       </c>
@@ -3877,7 +3877,7 @@
         <v>223</v>
       </c>
     </row>
-    <row r="189" spans="1:4" x14ac:dyDescent="0.2">
+    <row r="189" spans="1:4" x14ac:dyDescent="0.3">
       <c r="A189" s="1">
         <v>187</v>
       </c>
@@ -3891,7 +3891,7 @@
         <v>221</v>
       </c>
     </row>
-    <row r="190" spans="1:4" x14ac:dyDescent="0.2">
+    <row r="190" spans="1:4" x14ac:dyDescent="0.3">
       <c r="A190" s="1">
         <v>188</v>
       </c>
@@ -3905,7 +3905,7 @@
         <v>221</v>
       </c>
     </row>
-    <row r="191" spans="1:4" x14ac:dyDescent="0.2">
+    <row r="191" spans="1:4" x14ac:dyDescent="0.3">
       <c r="A191" s="1">
         <v>189</v>
       </c>
@@ -3919,7 +3919,7 @@
         <v>221</v>
       </c>
     </row>
-    <row r="192" spans="1:4" x14ac:dyDescent="0.2">
+    <row r="192" spans="1:4" x14ac:dyDescent="0.3">
       <c r="A192" s="1">
         <v>190</v>
       </c>
@@ -3933,7 +3933,7 @@
         <v>221</v>
       </c>
     </row>
-    <row r="193" spans="1:4" x14ac:dyDescent="0.2">
+    <row r="193" spans="1:4" x14ac:dyDescent="0.3">
       <c r="A193" s="1">
         <v>191</v>
       </c>
@@ -3947,7 +3947,7 @@
         <v>221</v>
       </c>
     </row>
-    <row r="194" spans="1:4" x14ac:dyDescent="0.2">
+    <row r="194" spans="1:4" x14ac:dyDescent="0.3">
       <c r="A194" s="1">
         <v>192</v>
       </c>
@@ -3961,7 +3961,7 @@
         <v>221</v>
       </c>
     </row>
-    <row r="195" spans="1:4" x14ac:dyDescent="0.2">
+    <row r="195" spans="1:4" x14ac:dyDescent="0.3">
       <c r="A195" s="1">
         <v>193</v>
       </c>
@@ -3975,7 +3975,7 @@
         <v>221</v>
       </c>
     </row>
-    <row r="196" spans="1:4" x14ac:dyDescent="0.2">
+    <row r="196" spans="1:4" x14ac:dyDescent="0.3">
       <c r="A196" s="1">
         <v>194</v>
       </c>
@@ -3989,7 +3989,7 @@
         <v>221</v>
       </c>
     </row>
-    <row r="197" spans="1:4" x14ac:dyDescent="0.2">
+    <row r="197" spans="1:4" x14ac:dyDescent="0.3">
       <c r="A197" s="1">
         <v>195</v>
       </c>
@@ -4003,7 +4003,7 @@
         <v>221</v>
       </c>
     </row>
-    <row r="198" spans="1:4" x14ac:dyDescent="0.2">
+    <row r="198" spans="1:4" x14ac:dyDescent="0.3">
       <c r="A198" s="1">
         <v>196</v>
       </c>
@@ -4017,7 +4017,7 @@
         <v>221</v>
       </c>
     </row>
-    <row r="199" spans="1:4" x14ac:dyDescent="0.2">
+    <row r="199" spans="1:4" x14ac:dyDescent="0.3">
       <c r="A199" s="1">
         <v>197</v>
       </c>
@@ -4031,7 +4031,7 @@
         <v>222</v>
       </c>
     </row>
-    <row r="200" spans="1:4" x14ac:dyDescent="0.2">
+    <row r="200" spans="1:4" x14ac:dyDescent="0.3">
       <c r="A200" s="1">
         <v>198</v>
       </c>
@@ -4045,7 +4045,7 @@
         <v>220</v>
       </c>
     </row>
-    <row r="201" spans="1:4" x14ac:dyDescent="0.2">
+    <row r="201" spans="1:4" x14ac:dyDescent="0.3">
       <c r="A201" s="1">
         <v>199</v>
       </c>
@@ -4059,7 +4059,7 @@
         <v>223</v>
       </c>
     </row>
-    <row r="202" spans="1:4" x14ac:dyDescent="0.2">
+    <row r="202" spans="1:4" x14ac:dyDescent="0.3">
       <c r="A202" s="1">
         <v>200</v>
       </c>
@@ -4073,7 +4073,7 @@
         <v>221</v>
       </c>
     </row>
-    <row r="203" spans="1:4" x14ac:dyDescent="0.2">
+    <row r="203" spans="1:4" x14ac:dyDescent="0.3">
       <c r="A203" s="1">
         <v>201</v>
       </c>
@@ -4087,7 +4087,7 @@
         <v>221</v>
       </c>
     </row>
-    <row r="204" spans="1:4" x14ac:dyDescent="0.2">
+    <row r="204" spans="1:4" x14ac:dyDescent="0.3">
       <c r="A204" s="1">
         <v>202</v>
       </c>
@@ -4101,7 +4101,7 @@
         <v>221</v>
       </c>
     </row>
-    <row r="205" spans="1:4" x14ac:dyDescent="0.2">
+    <row r="205" spans="1:4" x14ac:dyDescent="0.3">
       <c r="A205" s="1">
         <v>203</v>
       </c>
@@ -4115,7 +4115,7 @@
         <v>221</v>
       </c>
     </row>
-    <row r="206" spans="1:4" x14ac:dyDescent="0.2">
+    <row r="206" spans="1:4" x14ac:dyDescent="0.3">
       <c r="A206" s="1">
         <v>204</v>
       </c>
@@ -4129,7 +4129,7 @@
         <v>222</v>
       </c>
     </row>
-    <row r="207" spans="1:4" x14ac:dyDescent="0.2">
+    <row r="207" spans="1:4" x14ac:dyDescent="0.3">
       <c r="A207" s="1">
         <v>205</v>
       </c>
@@ -4143,7 +4143,7 @@
         <v>220</v>
       </c>
     </row>
-    <row r="208" spans="1:4" x14ac:dyDescent="0.2">
+    <row r="208" spans="1:4" x14ac:dyDescent="0.3">
       <c r="A208" s="1">
         <v>206</v>
       </c>
@@ -4157,7 +4157,7 @@
         <v>223</v>
       </c>
     </row>
-    <row r="209" spans="1:4" x14ac:dyDescent="0.2">
+    <row r="209" spans="1:4" x14ac:dyDescent="0.3">
       <c r="A209" s="1">
         <v>207</v>
       </c>
@@ -4171,7 +4171,7 @@
         <v>221</v>
       </c>
     </row>
-    <row r="210" spans="1:4" x14ac:dyDescent="0.2">
+    <row r="210" spans="1:4" x14ac:dyDescent="0.3">
       <c r="A210" s="1">
         <v>208</v>
       </c>
@@ -4185,7 +4185,7 @@
         <v>221</v>
       </c>
     </row>
-    <row r="211" spans="1:4" x14ac:dyDescent="0.2">
+    <row r="211" spans="1:4" x14ac:dyDescent="0.3">
       <c r="A211" s="1">
         <v>209</v>
       </c>
@@ -4199,7 +4199,7 @@
         <v>221</v>
       </c>
     </row>
-    <row r="212" spans="1:4" x14ac:dyDescent="0.2">
+    <row r="212" spans="1:4" x14ac:dyDescent="0.3">
       <c r="A212" s="1">
         <v>210</v>
       </c>
@@ -4213,7 +4213,7 @@
         <v>221</v>
       </c>
     </row>
-    <row r="213" spans="1:4" x14ac:dyDescent="0.2">
+    <row r="213" spans="1:4" x14ac:dyDescent="0.3">
       <c r="A213" s="1">
         <v>211</v>
       </c>
@@ -4227,7 +4227,7 @@
         <v>221</v>
       </c>
     </row>
-    <row r="214" spans="1:4" x14ac:dyDescent="0.2">
+    <row r="214" spans="1:4" x14ac:dyDescent="0.3">
       <c r="A214" s="1">
         <v>212</v>
       </c>
@@ -4241,7 +4241,7 @@
         <v>221</v>
       </c>
     </row>
-    <row r="215" spans="1:4" x14ac:dyDescent="0.2">
+    <row r="215" spans="1:4" x14ac:dyDescent="0.3">
       <c r="A215" s="1">
         <v>213</v>
       </c>
@@ -4255,7 +4255,7 @@
         <v>221</v>
       </c>
     </row>
-    <row r="216" spans="1:4" x14ac:dyDescent="0.2">
+    <row r="216" spans="1:4" x14ac:dyDescent="0.3">
       <c r="A216" s="1">
         <v>214</v>
       </c>
@@ -4269,7 +4269,7 @@
         <v>221</v>
       </c>
     </row>
-    <row r="217" spans="1:4" x14ac:dyDescent="0.2">
+    <row r="217" spans="1:4" x14ac:dyDescent="0.3">
       <c r="A217" s="1">
         <v>215</v>
       </c>
@@ -4283,7 +4283,7 @@
         <v>222</v>
       </c>
     </row>
-    <row r="218" spans="1:4" x14ac:dyDescent="0.2">
+    <row r="218" spans="1:4" x14ac:dyDescent="0.3">
       <c r="A218" s="1">
         <v>216</v>
       </c>
@@ -4297,7 +4297,7 @@
         <v>220</v>
       </c>
     </row>
-    <row r="219" spans="1:4" x14ac:dyDescent="0.2">
+    <row r="219" spans="1:4" x14ac:dyDescent="0.3">
       <c r="A219" s="1">
         <v>217</v>
       </c>
@@ -4311,7 +4311,7 @@
         <v>223</v>
       </c>
     </row>
-    <row r="220" spans="1:4" x14ac:dyDescent="0.2">
+    <row r="220" spans="1:4" x14ac:dyDescent="0.3">
       <c r="A220" s="1">
         <v>218</v>
       </c>
@@ -4325,7 +4325,7 @@
         <v>220</v>
       </c>
     </row>
-    <row r="221" spans="1:4" x14ac:dyDescent="0.2">
+    <row r="221" spans="1:4" x14ac:dyDescent="0.3">
       <c r="A221" s="1">
         <v>219</v>
       </c>
@@ -4339,7 +4339,7 @@
         <v>220</v>
       </c>
     </row>
-    <row r="222" spans="1:4" x14ac:dyDescent="0.2">
+    <row r="222" spans="1:4" x14ac:dyDescent="0.3">
       <c r="A222" s="1">
         <v>220</v>
       </c>
@@ -4353,7 +4353,7 @@
         <v>223</v>
       </c>
     </row>
-    <row r="223" spans="1:4" x14ac:dyDescent="0.2">
+    <row r="223" spans="1:4" x14ac:dyDescent="0.3">
       <c r="A223" s="1">
         <v>221</v>
       </c>
@@ -4367,7 +4367,7 @@
         <v>220</v>
       </c>
     </row>
-    <row r="224" spans="1:4" x14ac:dyDescent="0.2">
+    <row r="224" spans="1:4" x14ac:dyDescent="0.3">
       <c r="A224" s="1">
         <v>222</v>
       </c>
@@ -4381,7 +4381,7 @@
         <v>221</v>
       </c>
     </row>
-    <row r="225" spans="1:4" x14ac:dyDescent="0.2">
+    <row r="225" spans="1:4" x14ac:dyDescent="0.3">
       <c r="A225" s="1">
         <v>223</v>
       </c>
@@ -4395,7 +4395,7 @@
         <v>221</v>
       </c>
     </row>
-    <row r="226" spans="1:4" x14ac:dyDescent="0.2">
+    <row r="226" spans="1:4" x14ac:dyDescent="0.3">
       <c r="A226" s="1">
         <v>224</v>
       </c>
@@ -4409,7 +4409,7 @@
         <v>221</v>
       </c>
     </row>
-    <row r="227" spans="1:4" x14ac:dyDescent="0.2">
+    <row r="227" spans="1:4" x14ac:dyDescent="0.3">
       <c r="A227" s="1">
         <v>225</v>
       </c>
@@ -4423,7 +4423,7 @@
         <v>221</v>
       </c>
     </row>
-    <row r="228" spans="1:4" x14ac:dyDescent="0.2">
+    <row r="228" spans="1:4" x14ac:dyDescent="0.3">
       <c r="A228" s="1">
         <v>226</v>
       </c>
@@ -4437,7 +4437,7 @@
         <v>221</v>
       </c>
     </row>
-    <row r="229" spans="1:4" x14ac:dyDescent="0.2">
+    <row r="229" spans="1:4" x14ac:dyDescent="0.3">
       <c r="A229" s="1">
         <v>227</v>
       </c>
@@ -4451,7 +4451,7 @@
         <v>221</v>
       </c>
     </row>
-    <row r="230" spans="1:4" x14ac:dyDescent="0.2">
+    <row r="230" spans="1:4" x14ac:dyDescent="0.3">
       <c r="A230" s="1">
         <v>228</v>
       </c>
@@ -4465,7 +4465,7 @@
         <v>221</v>
       </c>
     </row>
-    <row r="231" spans="1:4" x14ac:dyDescent="0.2">
+    <row r="231" spans="1:4" x14ac:dyDescent="0.3">
       <c r="A231" s="1">
         <v>229</v>
       </c>
@@ -4479,7 +4479,7 @@
         <v>221</v>
       </c>
     </row>
-    <row r="232" spans="1:4" x14ac:dyDescent="0.2">
+    <row r="232" spans="1:4" x14ac:dyDescent="0.3">
       <c r="A232" s="1">
         <v>230</v>
       </c>
@@ -4503,12 +4503,12 @@
   <dimension ref="A1:F13"/>
   <sheetViews>
     <sheetView workbookViewId="0">
-      <selection activeCell="D28" sqref="D28"/>
+      <selection activeCell="A2" sqref="A2:B11"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr baseColWidth="10" defaultColWidth="8.83203125" defaultRowHeight="15" x14ac:dyDescent="0.2"/>
+  <sheetFormatPr defaultColWidth="8.77734375" defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
   <sheetData>
-    <row r="1" spans="1:6" x14ac:dyDescent="0.2">
+    <row r="1" spans="1:6" x14ac:dyDescent="0.3">
       <c r="B1" s="1" t="s">
         <v>3</v>
       </c>
@@ -4525,7 +4525,7 @@
         <v>10</v>
       </c>
     </row>
-    <row r="2" spans="1:6" x14ac:dyDescent="0.2">
+    <row r="2" spans="1:6" x14ac:dyDescent="0.3">
       <c r="A2" s="1">
         <v>0</v>
       </c>
@@ -4542,7 +4542,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="3" spans="1:6" x14ac:dyDescent="0.2">
+    <row r="3" spans="1:6" x14ac:dyDescent="0.3">
       <c r="A3" s="1">
         <v>1</v>
       </c>
@@ -4559,7 +4559,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="4" spans="1:6" x14ac:dyDescent="0.2">
+    <row r="4" spans="1:6" x14ac:dyDescent="0.3">
       <c r="A4" s="1">
         <v>2</v>
       </c>
@@ -4576,7 +4576,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="5" spans="1:6" x14ac:dyDescent="0.2">
+    <row r="5" spans="1:6" x14ac:dyDescent="0.3">
       <c r="A5" s="1">
         <v>3</v>
       </c>
@@ -4593,7 +4593,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="6" spans="1:6" x14ac:dyDescent="0.2">
+    <row r="6" spans="1:6" x14ac:dyDescent="0.3">
       <c r="A6" s="1">
         <v>4</v>
       </c>
@@ -4610,7 +4610,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="7" spans="1:6" x14ac:dyDescent="0.2">
+    <row r="7" spans="1:6" x14ac:dyDescent="0.3">
       <c r="A7" s="1">
         <v>5</v>
       </c>
@@ -4627,7 +4627,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="8" spans="1:6" x14ac:dyDescent="0.2">
+    <row r="8" spans="1:6" x14ac:dyDescent="0.3">
       <c r="A8" s="1">
         <v>6</v>
       </c>
@@ -4644,7 +4644,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="9" spans="1:6" x14ac:dyDescent="0.2">
+    <row r="9" spans="1:6" x14ac:dyDescent="0.3">
       <c r="A9" s="1">
         <v>7</v>
       </c>
@@ -4661,7 +4661,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="10" spans="1:6" x14ac:dyDescent="0.2">
+    <row r="10" spans="1:6" x14ac:dyDescent="0.3">
       <c r="A10" s="1">
         <v>8</v>
       </c>
@@ -4678,7 +4678,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="11" spans="1:6" x14ac:dyDescent="0.2">
+    <row r="11" spans="1:6" x14ac:dyDescent="0.3">
       <c r="A11" s="1">
         <v>9</v>
       </c>
@@ -4695,10 +4695,10 @@
         <v>1</v>
       </c>
     </row>
-    <row r="12" spans="1:6" x14ac:dyDescent="0.2">
+    <row r="12" spans="1:6" x14ac:dyDescent="0.3">
       <c r="A12" s="1"/>
     </row>
-    <row r="13" spans="1:6" x14ac:dyDescent="0.2">
+    <row r="13" spans="1:6" x14ac:dyDescent="0.3">
       <c r="A13" s="1"/>
     </row>
   </sheetData>
@@ -4712,9 +4712,9 @@
   <sheetViews>
     <sheetView workbookViewId="0"/>
   </sheetViews>
-  <sheetFormatPr baseColWidth="10" defaultColWidth="8.83203125" defaultRowHeight="15" x14ac:dyDescent="0.2"/>
+  <sheetFormatPr defaultColWidth="8.77734375" defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
   <sheetData>
-    <row r="1" spans="1:15" x14ac:dyDescent="0.2">
+    <row r="1" spans="1:15" x14ac:dyDescent="0.3">
       <c r="B1" s="1" t="s">
         <v>3</v>
       </c>
@@ -4758,7 +4758,7 @@
         <v>10</v>
       </c>
     </row>
-    <row r="2" spans="1:15" x14ac:dyDescent="0.2">
+    <row r="2" spans="1:15" x14ac:dyDescent="0.3">
       <c r="A2" s="1">
         <v>0</v>
       </c>
@@ -4805,7 +4805,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="3" spans="1:15" x14ac:dyDescent="0.2">
+    <row r="3" spans="1:15" x14ac:dyDescent="0.3">
       <c r="A3" s="1">
         <v>1</v>
       </c>
@@ -4852,7 +4852,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="4" spans="1:15" x14ac:dyDescent="0.2">
+    <row r="4" spans="1:15" x14ac:dyDescent="0.3">
       <c r="A4" s="1">
         <v>2</v>
       </c>
@@ -4899,7 +4899,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="5" spans="1:15" x14ac:dyDescent="0.2">
+    <row r="5" spans="1:15" x14ac:dyDescent="0.3">
       <c r="A5" s="1">
         <v>3</v>
       </c>
@@ -4946,7 +4946,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="6" spans="1:15" x14ac:dyDescent="0.2">
+    <row r="6" spans="1:15" x14ac:dyDescent="0.3">
       <c r="A6" s="1">
         <v>4</v>
       </c>
@@ -4993,7 +4993,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="7" spans="1:15" x14ac:dyDescent="0.2">
+    <row r="7" spans="1:15" x14ac:dyDescent="0.3">
       <c r="A7" s="1">
         <v>5</v>
       </c>
@@ -5040,7 +5040,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="8" spans="1:15" x14ac:dyDescent="0.2">
+    <row r="8" spans="1:15" x14ac:dyDescent="0.3">
       <c r="A8" s="1">
         <v>6</v>
       </c>
@@ -5087,7 +5087,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="9" spans="1:15" x14ac:dyDescent="0.2">
+    <row r="9" spans="1:15" x14ac:dyDescent="0.3">
       <c r="A9" s="1">
         <v>7</v>
       </c>
@@ -5145,9 +5145,9 @@
   <sheetViews>
     <sheetView workbookViewId="0"/>
   </sheetViews>
-  <sheetFormatPr baseColWidth="10" defaultColWidth="8.83203125" defaultRowHeight="15" x14ac:dyDescent="0.2"/>
+  <sheetFormatPr defaultColWidth="8.77734375" defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
   <sheetData>
-    <row r="1" spans="1:9" x14ac:dyDescent="0.2">
+    <row r="1" spans="1:9" x14ac:dyDescent="0.3">
       <c r="B1" s="1" t="s">
         <v>22</v>
       </c>
@@ -5173,7 +5173,7 @@
         <v>56</v>
       </c>
     </row>
-    <row r="2" spans="1:9" x14ac:dyDescent="0.2">
+    <row r="2" spans="1:9" x14ac:dyDescent="0.3">
       <c r="A2" s="1">
         <v>0</v>
       </c>
@@ -5196,7 +5196,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="3" spans="1:9" x14ac:dyDescent="0.2">
+    <row r="3" spans="1:9" x14ac:dyDescent="0.3">
       <c r="A3" s="1">
         <v>1</v>
       </c>
@@ -5219,7 +5219,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="4" spans="1:9" x14ac:dyDescent="0.2">
+    <row r="4" spans="1:9" x14ac:dyDescent="0.3">
       <c r="A4" s="1">
         <v>2</v>
       </c>
@@ -5242,7 +5242,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="5" spans="1:9" x14ac:dyDescent="0.2">
+    <row r="5" spans="1:9" x14ac:dyDescent="0.3">
       <c r="A5" s="1">
         <v>3</v>
       </c>
@@ -5265,7 +5265,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="6" spans="1:9" x14ac:dyDescent="0.2">
+    <row r="6" spans="1:9" x14ac:dyDescent="0.3">
       <c r="A6" s="1">
         <v>4</v>
       </c>
@@ -5288,7 +5288,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="7" spans="1:9" x14ac:dyDescent="0.2">
+    <row r="7" spans="1:9" x14ac:dyDescent="0.3">
       <c r="A7" s="1">
         <v>5</v>
       </c>
@@ -5311,7 +5311,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="8" spans="1:9" x14ac:dyDescent="0.2">
+    <row r="8" spans="1:9" x14ac:dyDescent="0.3">
       <c r="A8" s="1">
         <v>6</v>
       </c>
@@ -5334,7 +5334,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="9" spans="1:9" x14ac:dyDescent="0.2">
+    <row r="9" spans="1:9" x14ac:dyDescent="0.3">
       <c r="A9" s="1">
         <v>7</v>
       </c>
@@ -5370,9 +5370,9 @@
       <selection activeCell="A2" sqref="A2:K2"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr baseColWidth="10" defaultColWidth="8.83203125" defaultRowHeight="15" x14ac:dyDescent="0.2"/>
+  <sheetFormatPr defaultColWidth="8.77734375" defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
   <sheetData>
-    <row r="1" spans="1:9" x14ac:dyDescent="0.2">
+    <row r="1" spans="1:9" x14ac:dyDescent="0.3">
       <c r="B1" s="1" t="s">
         <v>22</v>
       </c>
@@ -5398,7 +5398,7 @@
         <v>10</v>
       </c>
     </row>
-    <row r="2" spans="1:9" x14ac:dyDescent="0.2">
+    <row r="2" spans="1:9" x14ac:dyDescent="0.3">
       <c r="A2" s="1"/>
     </row>
   </sheetData>
@@ -5414,9 +5414,9 @@
       <selection activeCell="A2" sqref="A2:XFD5"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr baseColWidth="10" defaultColWidth="8.83203125" defaultRowHeight="15" x14ac:dyDescent="0.2"/>
+  <sheetFormatPr defaultColWidth="8.77734375" defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
   <sheetData>
-    <row r="1" spans="1:10" x14ac:dyDescent="0.2">
+    <row r="1" spans="1:10" x14ac:dyDescent="0.3">
       <c r="B1" s="1" t="s">
         <v>3</v>
       </c>
@@ -5445,10 +5445,10 @@
         <v>10</v>
       </c>
     </row>
-    <row r="2" spans="1:10" x14ac:dyDescent="0.2">
+    <row r="2" spans="1:10" x14ac:dyDescent="0.3">
       <c r="A2" s="1"/>
     </row>
-    <row r="3" spans="1:10" x14ac:dyDescent="0.2">
+    <row r="3" spans="1:10" x14ac:dyDescent="0.3">
       <c r="A3" s="1"/>
     </row>
   </sheetData>
@@ -5464,9 +5464,9 @@
       <selection activeCell="A2" sqref="A2:XFD3"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr baseColWidth="10" defaultColWidth="8.83203125" defaultRowHeight="15" x14ac:dyDescent="0.2"/>
+  <sheetFormatPr defaultColWidth="8.77734375" defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
   <sheetData>
-    <row r="1" spans="1:15" x14ac:dyDescent="0.2">
+    <row r="1" spans="1:15" x14ac:dyDescent="0.3">
       <c r="B1" s="1" t="s">
         <v>3</v>
       </c>
@@ -5510,10 +5510,10 @@
         <v>10</v>
       </c>
     </row>
-    <row r="2" spans="1:15" x14ac:dyDescent="0.2">
+    <row r="2" spans="1:15" x14ac:dyDescent="0.3">
       <c r="A2" s="1"/>
     </row>
-    <row r="3" spans="1:15" x14ac:dyDescent="0.2">
+    <row r="3" spans="1:15" x14ac:dyDescent="0.3">
       <c r="A3" s="1"/>
     </row>
   </sheetData>
@@ -5523,15 +5523,15 @@
 
 <file path=xl/worksheets/sheet8.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-1300-000000000000}">
-  <dimension ref="A1:D3"/>
+  <dimension ref="A1:E11"/>
   <sheetViews>
-    <sheetView workbookViewId="0">
-      <selection activeCell="O18" sqref="O18"/>
+    <sheetView tabSelected="1" workbookViewId="0">
+      <selection activeCell="C12" sqref="C12"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr baseColWidth="10" defaultColWidth="8.83203125" defaultRowHeight="15" x14ac:dyDescent="0.2"/>
+  <sheetFormatPr defaultColWidth="8.77734375" defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
   <sheetData>
-    <row r="1" spans="1:4" x14ac:dyDescent="0.2">
+    <row r="1" spans="1:5" x14ac:dyDescent="0.3">
       <c r="B1" s="1" t="s">
         <v>139</v>
       </c>
@@ -5542,19 +5542,125 @@
         <v>141</v>
       </c>
     </row>
-    <row r="2" spans="1:4" x14ac:dyDescent="0.2">
+    <row r="2" spans="1:5" x14ac:dyDescent="0.3">
       <c r="A2" s="1">
         <v>0</v>
       </c>
       <c r="B2">
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="C2">
         <v>0</v>
       </c>
-    </row>
-    <row r="3" spans="1:4" x14ac:dyDescent="0.2">
-      <c r="A3" s="1"/>
+      <c r="E2" s="1"/>
+    </row>
+    <row r="3" spans="1:5" x14ac:dyDescent="0.3">
+      <c r="A3" s="1">
+        <v>1</v>
+      </c>
+      <c r="B3">
+        <v>1</v>
+      </c>
+      <c r="C3">
+        <v>1</v>
+      </c>
+      <c r="E3" s="1"/>
+    </row>
+    <row r="4" spans="1:5" x14ac:dyDescent="0.3">
+      <c r="A4" s="1">
+        <v>2</v>
+      </c>
+      <c r="B4">
+        <v>0</v>
+      </c>
+      <c r="C4">
+        <v>2</v>
+      </c>
+      <c r="E4" s="1"/>
+    </row>
+    <row r="5" spans="1:5" x14ac:dyDescent="0.3">
+      <c r="A5" s="1">
+        <v>3</v>
+      </c>
+      <c r="B5">
+        <v>0</v>
+      </c>
+      <c r="C5">
+        <v>3</v>
+      </c>
+      <c r="E5" s="1"/>
+    </row>
+    <row r="6" spans="1:5" x14ac:dyDescent="0.3">
+      <c r="A6" s="1">
+        <v>4</v>
+      </c>
+      <c r="B6">
+        <v>0</v>
+      </c>
+      <c r="C6">
+        <v>4</v>
+      </c>
+      <c r="E6" s="1"/>
+    </row>
+    <row r="7" spans="1:5" x14ac:dyDescent="0.3">
+      <c r="A7" s="1">
+        <v>5</v>
+      </c>
+      <c r="B7">
+        <v>0</v>
+      </c>
+      <c r="C7">
+        <v>5</v>
+      </c>
+      <c r="E7" s="1"/>
+    </row>
+    <row r="8" spans="1:5" x14ac:dyDescent="0.3">
+      <c r="A8" s="1">
+        <v>6</v>
+      </c>
+      <c r="B8">
+        <v>0</v>
+      </c>
+      <c r="C8">
+        <v>6</v>
+      </c>
+      <c r="E8" s="1"/>
+    </row>
+    <row r="9" spans="1:5" x14ac:dyDescent="0.3">
+      <c r="A9" s="1">
+        <v>7</v>
+      </c>
+      <c r="B9">
+        <v>0</v>
+      </c>
+      <c r="C9">
+        <v>7</v>
+      </c>
+      <c r="E9" s="1"/>
+    </row>
+    <row r="10" spans="1:5" x14ac:dyDescent="0.3">
+      <c r="A10" s="1">
+        <v>8</v>
+      </c>
+      <c r="B10">
+        <v>2</v>
+      </c>
+      <c r="C10">
+        <v>2</v>
+      </c>
+      <c r="E10" s="1"/>
+    </row>
+    <row r="11" spans="1:5" x14ac:dyDescent="0.3">
+      <c r="A11" s="1">
+        <v>9</v>
+      </c>
+      <c r="B11">
+        <v>2</v>
+      </c>
+      <c r="C11">
+        <v>3</v>
+      </c>
+      <c r="E11" s="1"/>
     </row>
   </sheetData>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
@@ -5567,9 +5673,9 @@
   <sheetViews>
     <sheetView workbookViewId="0"/>
   </sheetViews>
-  <sheetFormatPr baseColWidth="10" defaultColWidth="8.83203125" defaultRowHeight="15" x14ac:dyDescent="0.2"/>
+  <sheetFormatPr defaultColWidth="8.77734375" defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
   <sheetData>
-    <row r="1" spans="1:8" x14ac:dyDescent="0.2">
+    <row r="1" spans="1:8" x14ac:dyDescent="0.3">
       <c r="B1" s="1" t="s">
         <v>74</v>
       </c>
@@ -5592,7 +5698,7 @@
         <v>143</v>
       </c>
     </row>
-    <row r="2" spans="1:8" x14ac:dyDescent="0.2">
+    <row r="2" spans="1:8" x14ac:dyDescent="0.3">
       <c r="A2" s="1" t="s">
         <v>144</v>
       </c>
@@ -5618,7 +5724,7 @@
         <v>4.0299999999999997E-3</v>
       </c>
     </row>
-    <row r="3" spans="1:8" x14ac:dyDescent="0.2">
+    <row r="3" spans="1:8" x14ac:dyDescent="0.3">
       <c r="A3" s="1" t="s">
         <v>145</v>
       </c>
@@ -5644,7 +5750,7 @@
         <v>4.0299999999999997E-3</v>
       </c>
     </row>
-    <row r="4" spans="1:8" x14ac:dyDescent="0.2">
+    <row r="4" spans="1:8" x14ac:dyDescent="0.3">
       <c r="A4" s="1" t="s">
         <v>146</v>
       </c>
@@ -5670,7 +5776,7 @@
         <v>4.0299999999999997E-3</v>
       </c>
     </row>
-    <row r="5" spans="1:8" x14ac:dyDescent="0.2">
+    <row r="5" spans="1:8" x14ac:dyDescent="0.3">
       <c r="A5" s="1" t="s">
         <v>147</v>
       </c>
@@ -5696,7 +5802,7 @@
         <v>4.0299999999999997E-3</v>
       </c>
     </row>
-    <row r="6" spans="1:8" x14ac:dyDescent="0.2">
+    <row r="6" spans="1:8" x14ac:dyDescent="0.3">
       <c r="A6" s="1" t="s">
         <v>148</v>
       </c>
@@ -5722,7 +5828,7 @@
         <v>4.0299999999999997E-3</v>
       </c>
     </row>
-    <row r="7" spans="1:8" x14ac:dyDescent="0.2">
+    <row r="7" spans="1:8" x14ac:dyDescent="0.3">
       <c r="A7" s="1" t="s">
         <v>149</v>
       </c>
@@ -5748,7 +5854,7 @@
         <v>4.0299999999999997E-3</v>
       </c>
     </row>
-    <row r="8" spans="1:8" x14ac:dyDescent="0.2">
+    <row r="8" spans="1:8" x14ac:dyDescent="0.3">
       <c r="A8" s="1" t="s">
         <v>150</v>
       </c>
@@ -5774,7 +5880,7 @@
         <v>4.0299999999999997E-3</v>
       </c>
     </row>
-    <row r="9" spans="1:8" x14ac:dyDescent="0.2">
+    <row r="9" spans="1:8" x14ac:dyDescent="0.3">
       <c r="A9" s="1" t="s">
         <v>151</v>
       </c>
@@ -5800,7 +5906,7 @@
         <v>4.0299999999999997E-3</v>
       </c>
     </row>
-    <row r="10" spans="1:8" x14ac:dyDescent="0.2">
+    <row r="10" spans="1:8" x14ac:dyDescent="0.3">
       <c r="A10" s="1" t="s">
         <v>152</v>
       </c>
@@ -5826,7 +5932,7 @@
         <v>4.0299999999999997E-3</v>
       </c>
     </row>
-    <row r="11" spans="1:8" x14ac:dyDescent="0.2">
+    <row r="11" spans="1:8" x14ac:dyDescent="0.3">
       <c r="A11" s="1" t="s">
         <v>153</v>
       </c>
@@ -5852,7 +5958,7 @@
         <v>4.0299999999999997E-3</v>
       </c>
     </row>
-    <row r="12" spans="1:8" x14ac:dyDescent="0.2">
+    <row r="12" spans="1:8" x14ac:dyDescent="0.3">
       <c r="A12" s="1" t="s">
         <v>154</v>
       </c>
@@ -5878,7 +5984,7 @@
         <v>4.0299999999999997E-3</v>
       </c>
     </row>
-    <row r="13" spans="1:8" x14ac:dyDescent="0.2">
+    <row r="13" spans="1:8" x14ac:dyDescent="0.3">
       <c r="A13" s="1" t="s">
         <v>155</v>
       </c>
@@ -5904,7 +6010,7 @@
         <v>4.0299999999999997E-3</v>
       </c>
     </row>
-    <row r="14" spans="1:8" x14ac:dyDescent="0.2">
+    <row r="14" spans="1:8" x14ac:dyDescent="0.3">
       <c r="A14" s="1" t="s">
         <v>156</v>
       </c>
@@ -5930,7 +6036,7 @@
         <v>4.0299999999999997E-3</v>
       </c>
     </row>
-    <row r="15" spans="1:8" x14ac:dyDescent="0.2">
+    <row r="15" spans="1:8" x14ac:dyDescent="0.3">
       <c r="A15" s="1" t="s">
         <v>157</v>
       </c>
@@ -5956,7 +6062,7 @@
         <v>4.0299999999999997E-3</v>
       </c>
     </row>
-    <row r="16" spans="1:8" x14ac:dyDescent="0.2">
+    <row r="16" spans="1:8" x14ac:dyDescent="0.3">
       <c r="A16" s="1" t="s">
         <v>158</v>
       </c>
@@ -5982,7 +6088,7 @@
         <v>4.0299999999999997E-3</v>
       </c>
     </row>
-    <row r="17" spans="1:8" x14ac:dyDescent="0.2">
+    <row r="17" spans="1:8" x14ac:dyDescent="0.3">
       <c r="A17" s="1" t="s">
         <v>159</v>
       </c>
@@ -6008,7 +6114,7 @@
         <v>3.9300000000000003E-3</v>
       </c>
     </row>
-    <row r="18" spans="1:8" x14ac:dyDescent="0.2">
+    <row r="18" spans="1:8" x14ac:dyDescent="0.3">
       <c r="A18" s="1" t="s">
         <v>160</v>
       </c>
@@ -6034,7 +6140,7 @@
         <v>3.9300000000000003E-3</v>
       </c>
     </row>
-    <row r="19" spans="1:8" x14ac:dyDescent="0.2">
+    <row r="19" spans="1:8" x14ac:dyDescent="0.3">
       <c r="A19" s="1" t="s">
         <v>161</v>
       </c>
@@ -6060,7 +6166,7 @@
         <v>3.9300000000000003E-3</v>
       </c>
     </row>
-    <row r="20" spans="1:8" x14ac:dyDescent="0.2">
+    <row r="20" spans="1:8" x14ac:dyDescent="0.3">
       <c r="A20" s="1" t="s">
         <v>162</v>
       </c>
@@ -6086,7 +6192,7 @@
         <v>3.9300000000000003E-3</v>
       </c>
     </row>
-    <row r="21" spans="1:8" x14ac:dyDescent="0.2">
+    <row r="21" spans="1:8" x14ac:dyDescent="0.3">
       <c r="A21" s="1" t="s">
         <v>163</v>
       </c>
@@ -6112,7 +6218,7 @@
         <v>4.0299999999999997E-3</v>
       </c>
     </row>
-    <row r="22" spans="1:8" x14ac:dyDescent="0.2">
+    <row r="22" spans="1:8" x14ac:dyDescent="0.3">
       <c r="A22" s="1" t="s">
         <v>164</v>
       </c>
@@ -6138,7 +6244,7 @@
         <v>4.0299999999999997E-3</v>
       </c>
     </row>
-    <row r="23" spans="1:8" x14ac:dyDescent="0.2">
+    <row r="23" spans="1:8" x14ac:dyDescent="0.3">
       <c r="A23" s="1" t="s">
         <v>165</v>
       </c>
@@ -6164,7 +6270,7 @@
         <v>4.0299999999999997E-3</v>
       </c>
     </row>
-    <row r="24" spans="1:8" x14ac:dyDescent="0.2">
+    <row r="24" spans="1:8" x14ac:dyDescent="0.3">
       <c r="A24" s="1" t="s">
         <v>166</v>
       </c>
@@ -6190,7 +6296,7 @@
         <v>4.0299999999999997E-3</v>
       </c>
     </row>
-    <row r="25" spans="1:8" x14ac:dyDescent="0.2">
+    <row r="25" spans="1:8" x14ac:dyDescent="0.3">
       <c r="A25" s="1" t="s">
         <v>167</v>
       </c>
@@ -6216,7 +6322,7 @@
         <v>4.0299999999999997E-3</v>
       </c>
     </row>
-    <row r="26" spans="1:8" x14ac:dyDescent="0.2">
+    <row r="26" spans="1:8" x14ac:dyDescent="0.3">
       <c r="A26" s="1" t="s">
         <v>168</v>
       </c>
@@ -6242,7 +6348,7 @@
         <v>4.0299999999999997E-3</v>
       </c>
     </row>
-    <row r="27" spans="1:8" x14ac:dyDescent="0.2">
+    <row r="27" spans="1:8" x14ac:dyDescent="0.3">
       <c r="A27" s="1" t="s">
         <v>169</v>
       </c>
@@ -6268,7 +6374,7 @@
         <v>4.0299999999999997E-3</v>
       </c>
     </row>
-    <row r="28" spans="1:8" x14ac:dyDescent="0.2">
+    <row r="28" spans="1:8" x14ac:dyDescent="0.3">
       <c r="A28" s="1" t="s">
         <v>170</v>
       </c>
@@ -6294,7 +6400,7 @@
         <v>4.0299999999999997E-3</v>
       </c>
     </row>
-    <row r="29" spans="1:8" x14ac:dyDescent="0.2">
+    <row r="29" spans="1:8" x14ac:dyDescent="0.3">
       <c r="A29" s="1" t="s">
         <v>171</v>
       </c>
@@ -6320,7 +6426,7 @@
         <v>4.0299999999999997E-3</v>
       </c>
     </row>
-    <row r="30" spans="1:8" x14ac:dyDescent="0.2">
+    <row r="30" spans="1:8" x14ac:dyDescent="0.3">
       <c r="A30" s="1" t="s">
         <v>172</v>
       </c>
@@ -6346,7 +6452,7 @@
         <v>4.0299999999999997E-3</v>
       </c>
     </row>
-    <row r="31" spans="1:8" x14ac:dyDescent="0.2">
+    <row r="31" spans="1:8" x14ac:dyDescent="0.3">
       <c r="A31" s="1" t="s">
         <v>173</v>
       </c>
@@ -6372,7 +6478,7 @@
         <v>4.0299999999999997E-3</v>
       </c>
     </row>
-    <row r="32" spans="1:8" x14ac:dyDescent="0.2">
+    <row r="32" spans="1:8" x14ac:dyDescent="0.3">
       <c r="A32" s="1" t="s">
         <v>174</v>
       </c>
@@ -6398,7 +6504,7 @@
         <v>4.0299999999999997E-3</v>
       </c>
     </row>
-    <row r="33" spans="1:8" x14ac:dyDescent="0.2">
+    <row r="33" spans="1:8" x14ac:dyDescent="0.3">
       <c r="A33" s="1" t="s">
         <v>175</v>
       </c>
@@ -6424,7 +6530,7 @@
         <v>4.0299999999999997E-3</v>
       </c>
     </row>
-    <row r="34" spans="1:8" x14ac:dyDescent="0.2">
+    <row r="34" spans="1:8" x14ac:dyDescent="0.3">
       <c r="A34" s="1" t="s">
         <v>176</v>
       </c>
@@ -6450,7 +6556,7 @@
         <v>4.0299999999999997E-3</v>
       </c>
     </row>
-    <row r="35" spans="1:8" x14ac:dyDescent="0.2">
+    <row r="35" spans="1:8" x14ac:dyDescent="0.3">
       <c r="A35" s="1" t="s">
         <v>177</v>
       </c>
@@ -6476,7 +6582,7 @@
         <v>4.0299999999999997E-3</v>
       </c>
     </row>
-    <row r="36" spans="1:8" x14ac:dyDescent="0.2">
+    <row r="36" spans="1:8" x14ac:dyDescent="0.3">
       <c r="A36" s="1" t="s">
         <v>178</v>
       </c>
@@ -6502,7 +6608,7 @@
         <v>4.0299999999999997E-3</v>
       </c>
     </row>
-    <row r="37" spans="1:8" x14ac:dyDescent="0.2">
+    <row r="37" spans="1:8" x14ac:dyDescent="0.3">
       <c r="A37" s="1" t="s">
         <v>179</v>
       </c>
@@ -6528,7 +6634,7 @@
         <v>4.0299999999999997E-3</v>
       </c>
     </row>
-    <row r="38" spans="1:8" x14ac:dyDescent="0.2">
+    <row r="38" spans="1:8" x14ac:dyDescent="0.3">
       <c r="A38" s="1" t="s">
         <v>180</v>
       </c>
@@ -6554,7 +6660,7 @@
         <v>4.0299999999999997E-3</v>
       </c>
     </row>
-    <row r="39" spans="1:8" x14ac:dyDescent="0.2">
+    <row r="39" spans="1:8" x14ac:dyDescent="0.3">
       <c r="A39" s="1" t="s">
         <v>181</v>
       </c>
@@ -6580,7 +6686,7 @@
         <v>4.0299999999999997E-3</v>
       </c>
     </row>
-    <row r="40" spans="1:8" x14ac:dyDescent="0.2">
+    <row r="40" spans="1:8" x14ac:dyDescent="0.3">
       <c r="A40" s="1" t="s">
         <v>182</v>
       </c>
@@ -6606,7 +6712,7 @@
         <v>4.0299999999999997E-3</v>
       </c>
     </row>
-    <row r="41" spans="1:8" x14ac:dyDescent="0.2">
+    <row r="41" spans="1:8" x14ac:dyDescent="0.3">
       <c r="A41" s="1" t="s">
         <v>183</v>
       </c>
@@ -6632,7 +6738,7 @@
         <v>4.0299999999999997E-3</v>
       </c>
     </row>
-    <row r="42" spans="1:8" x14ac:dyDescent="0.2">
+    <row r="42" spans="1:8" x14ac:dyDescent="0.3">
       <c r="A42" s="1" t="s">
         <v>184</v>
       </c>
@@ -6658,7 +6764,7 @@
         <v>4.0299999999999997E-3</v>
       </c>
     </row>
-    <row r="43" spans="1:8" x14ac:dyDescent="0.2">
+    <row r="43" spans="1:8" x14ac:dyDescent="0.3">
       <c r="A43" s="1" t="s">
         <v>185</v>
       </c>
@@ -6684,7 +6790,7 @@
         <v>4.0299999999999997E-3</v>
       </c>
     </row>
-    <row r="44" spans="1:8" x14ac:dyDescent="0.2">
+    <row r="44" spans="1:8" x14ac:dyDescent="0.3">
       <c r="A44" s="1" t="s">
         <v>186</v>
       </c>
@@ -6710,7 +6816,7 @@
         <v>4.0299999999999997E-3</v>
       </c>
     </row>
-    <row r="45" spans="1:8" x14ac:dyDescent="0.2">
+    <row r="45" spans="1:8" x14ac:dyDescent="0.3">
       <c r="A45" s="1" t="s">
         <v>187</v>
       </c>
@@ -6736,7 +6842,7 @@
         <v>4.0299999999999997E-3</v>
       </c>
     </row>
-    <row r="46" spans="1:8" x14ac:dyDescent="0.2">
+    <row r="46" spans="1:8" x14ac:dyDescent="0.3">
       <c r="A46" s="1" t="s">
         <v>188</v>
       </c>
@@ -6762,7 +6868,7 @@
         <v>4.0299999999999997E-3</v>
       </c>
     </row>
-    <row r="47" spans="1:8" x14ac:dyDescent="0.2">
+    <row r="47" spans="1:8" x14ac:dyDescent="0.3">
       <c r="A47" s="1" t="s">
         <v>189</v>
       </c>
@@ -6788,7 +6894,7 @@
         <v>4.0299999999999997E-3</v>
       </c>
     </row>
-    <row r="48" spans="1:8" x14ac:dyDescent="0.2">
+    <row r="48" spans="1:8" x14ac:dyDescent="0.3">
       <c r="A48" s="1" t="s">
         <v>190</v>
       </c>
@@ -6814,7 +6920,7 @@
         <v>4.0299999999999997E-3</v>
       </c>
     </row>
-    <row r="49" spans="1:8" x14ac:dyDescent="0.2">
+    <row r="49" spans="1:8" x14ac:dyDescent="0.3">
       <c r="A49" s="1" t="s">
         <v>191</v>
       </c>
@@ -6840,7 +6946,7 @@
         <v>4.0299999999999997E-3</v>
       </c>
     </row>
-    <row r="50" spans="1:8" x14ac:dyDescent="0.2">
+    <row r="50" spans="1:8" x14ac:dyDescent="0.3">
       <c r="A50" s="1" t="s">
         <v>192</v>
       </c>
@@ -6866,7 +6972,7 @@
         <v>4.0299999999999997E-3</v>
       </c>
     </row>
-    <row r="51" spans="1:8" x14ac:dyDescent="0.2">
+    <row r="51" spans="1:8" x14ac:dyDescent="0.3">
       <c r="A51" s="1" t="s">
         <v>193</v>
       </c>
@@ -6892,7 +6998,7 @@
         <v>4.0299999999999997E-3</v>
       </c>
     </row>
-    <row r="52" spans="1:8" x14ac:dyDescent="0.2">
+    <row r="52" spans="1:8" x14ac:dyDescent="0.3">
       <c r="A52" s="1" t="s">
         <v>194</v>
       </c>
@@ -6918,7 +7024,7 @@
         <v>4.0299999999999997E-3</v>
       </c>
     </row>
-    <row r="53" spans="1:8" x14ac:dyDescent="0.2">
+    <row r="53" spans="1:8" x14ac:dyDescent="0.3">
       <c r="A53" s="1" t="s">
         <v>87</v>
       </c>
@@ -6941,7 +7047,7 @@
         <v>70</v>
       </c>
     </row>
-    <row r="54" spans="1:8" x14ac:dyDescent="0.2">
+    <row r="54" spans="1:8" x14ac:dyDescent="0.3">
       <c r="A54" s="1" t="s">
         <v>195</v>
       </c>
@@ -6964,7 +7070,7 @@
         <v>50</v>
       </c>
     </row>
-    <row r="55" spans="1:8" x14ac:dyDescent="0.2">
+    <row r="55" spans="1:8" x14ac:dyDescent="0.3">
       <c r="A55" s="1" t="s">
         <v>196</v>
       </c>
@@ -6987,7 +7093,7 @@
         <v>150</v>
       </c>
     </row>
-    <row r="56" spans="1:8" x14ac:dyDescent="0.2">
+    <row r="56" spans="1:8" x14ac:dyDescent="0.3">
       <c r="A56" s="1" t="s">
         <v>197</v>
       </c>
@@ -7010,7 +7116,7 @@
         <v>185</v>
       </c>
     </row>
-    <row r="57" spans="1:8" x14ac:dyDescent="0.2">
+    <row r="57" spans="1:8" x14ac:dyDescent="0.3">
       <c r="A57" s="1" t="s">
         <v>198</v>
       </c>

</xml_diff>